<commit_message>
almost finish topic 5 bivariate
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF4EC01-778D-4F23-A1CC-FCBC3504B145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EAEEA2-3E9F-47DF-86E4-E21617FB124C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="152">
   <si>
     <t>Assignment</t>
   </si>
@@ -226,9 +226,6 @@
     <t>Video</t>
   </si>
   <si>
-    <t>[HW05 Graphing Relationships](hw/05_bivariate_graphing_assignment.html)</t>
-  </si>
-  <si>
     <t>[Poster prep Stage I](project.html)</t>
   </si>
   <si>
@@ -263,9 +260,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>Describing relationships (Q~Q)</t>
   </si>
   <si>
     <t>T-tests for difference in means</t>
@@ -282,9 +276,6 @@
   </si>
   <si>
     <t>Develop Research Poster</t>
-  </si>
-  <si>
-    <t>Describing relationships (C~C, Q~C)</t>
   </si>
   <si>
     <t>[Poster prep Stage III](project.html)</t>
@@ -326,9 +317,6 @@
   </si>
   <si>
     <t>[Tidy data principles](https://tidyr.tidyverse.org/articles/tidy-data.html#tidying) (Optional)</t>
-  </si>
-  <si>
-    <t>[Lec04 - Describing Relationships (ASCN Ch 2.4)](https://norcalbiostat.github.io/AppliedStatistics_notes/bivariate-visualizations.html)</t>
   </si>
   <si>
     <t>Describing distributions of data</t>
@@ -403,9 +391,6 @@
   </si>
   <si>
     <t>Project Stage 1: Choosing your topic</t>
-  </si>
-  <si>
-    <t>t05_probability</t>
   </si>
   <si>
     <t>t06_estimation</t>
@@ -501,9 +486,6 @@
     <t>lec01-data_arch</t>
   </si>
   <si>
-    <t>lec04_describing_data</t>
-  </si>
-  <si>
     <t>[HW01 Data Entry](hw01-data_entry.html)</t>
   </si>
   <si>
@@ -514,6 +496,34 @@
   </si>
   <si>
     <t>[HW04 Univariate Graphing](hw04-univ_graphing.html)</t>
+  </si>
+  <si>
+    <t>t05-describing_relationships</t>
+  </si>
+  <si>
+    <t>t06-probability</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 4  
+ASCN Ch 2.4</t>
+  </si>
+  <si>
+    <t>lec05-describing_relationships</t>
+  </si>
+  <si>
+    <t>lec04-describing_data</t>
+  </si>
+  <si>
+    <t>[HW05 Graphing Relationships](hw05-biv_graphing.html)</t>
+  </si>
+  <si>
+    <t>Describing relationships between two varaibles</t>
+  </si>
+  <si>
+    <t>First step in investigating a question about an association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create appropriate summary statistics and visualizations for combinations of two measures. </t>
   </si>
 </sst>
 </file>
@@ -1402,9 +1412,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1423,28 +1433,28 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>106</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>110</v>
       </c>
       <c r="I1" s="34" t="s">
         <v>31</v>
@@ -1453,10 +1463,10 @@
         <v>59</v>
       </c>
       <c r="K1" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="37" t="s">
         <v>104</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1470,31 +1480,31 @@
         <v>43333</v>
       </c>
       <c r="D2" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="45" t="s">
+      <c r="G2" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="41" t="s">
+      <c r="J2" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="42" t="s">
         <v>105</v>
-      </c>
-      <c r="J2" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="K2" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="42" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="189" x14ac:dyDescent="0.25">
@@ -1505,29 +1515,29 @@
         <v>43333</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J3" s="46"/>
       <c r="K3" s="41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -1539,10 +1549,10 @@
       </c>
       <c r="D4" s="51"/>
       <c r="E4" s="55" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G4" s="51"/>
       <c r="H4" s="51"/>
@@ -1562,29 +1572,29 @@
         <v>43340</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I5" s="49" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J5" s="45"/>
       <c r="K5" s="41" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1595,29 +1605,29 @@
         <v>43342</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I6" s="45" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="J6" s="45"/>
       <c r="K6" s="41" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1632,10 +1642,10 @@
       </c>
       <c r="D7" s="46"/>
       <c r="E7" s="52" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G7" s="45"/>
       <c r="H7" s="45"/>
@@ -1655,27 +1665,27 @@
         <v>43354</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G8" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" s="45" t="s">
         <v>135</v>
-      </c>
-      <c r="H8" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="I8" s="45" t="s">
-        <v>140</v>
       </c>
       <c r="J8" s="45"/>
       <c r="K8" s="45"/>
       <c r="L8" s="42" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1696,37 +1706,52 @@
       <c r="J9" s="50"/>
       <c r="K9" s="51"/>
       <c r="L9" s="43" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>5</v>
+      </c>
+      <c r="B10" s="27">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="C10" s="44">
         <v>43361</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="41"/>
+      <c r="D10" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>151</v>
+      </c>
       <c r="H10" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="45"/>
+        <v>146</v>
+      </c>
+      <c r="I10" s="45" t="s">
+        <v>145</v>
+      </c>
       <c r="J10" s="45"/>
       <c r="K10" s="45"/>
       <c r="L10" s="29" t="s">
-        <v>60</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
+      <c r="A11" s="4">
+        <v>6</v>
+      </c>
+      <c r="B11" s="27">
+        <v>6.1</v>
+      </c>
       <c r="C11" s="31">
         <v>43368</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
@@ -1735,7 +1760,9 @@
       <c r="L11" s="29"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
+      <c r="B12" s="27">
+        <v>6.2</v>
+      </c>
       <c r="C12" s="31">
         <v>43370</v>
       </c>
@@ -1750,7 +1777,7 @@
       <c r="J12" s="38"/>
       <c r="K12" s="39"/>
       <c r="L12" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="173.25" x14ac:dyDescent="0.25">
@@ -1759,20 +1786,20 @@
         <v>43375</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>115</v>
+        <v>144</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J13" s="28"/>
       <c r="L13" s="40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1782,7 +1809,7 @@
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
@@ -1797,10 +1824,10 @@
         <v>43382</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
@@ -1814,17 +1841,17 @@
         <v>43384</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
       <c r="J16" s="28"/>
       <c r="L16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -1834,7 +1861,7 @@
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F17" s="28"/>
     </row>
@@ -1845,7 +1872,7 @@
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
@@ -1886,7 +1913,7 @@
       <c r="J20" s="38"/>
       <c r="K20" s="39"/>
       <c r="L20" s="38" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -1895,17 +1922,17 @@
         <v>43410</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F21" s="28"/>
       <c r="I21" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L21" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -1915,7 +1942,7 @@
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="28" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
@@ -1925,7 +1952,7 @@
       </c>
       <c r="J22" s="28"/>
       <c r="L22" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -1943,14 +1970,14 @@
       </c>
       <c r="J23" s="28"/>
       <c r="L23" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="27"/>
       <c r="C24" s="31"/>
       <c r="D24" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>29</v>
@@ -1979,7 +2006,7 @@
       <c r="J25" s="38"/>
       <c r="K25" s="39"/>
       <c r="L25" s="38" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -1991,10 +2018,10 @@
         <v>43431</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
@@ -2014,11 +2041,11 @@
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F27" s="28"/>
       <c r="L27" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -2027,10 +2054,10 @@
         <v>43440</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E28" s="48" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
@@ -2064,7 +2091,7 @@
         <v>6</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2748,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="21" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
work on probability and inference
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80EE39B-F57B-486F-8496-72F64B832382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA3C993-0CDB-4CFD-B3B4-02104866D658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="162">
   <si>
     <t>Assignment</t>
   </si>
@@ -174,9 +174,6 @@
     <t>05 PR</t>
   </si>
   <si>
-    <t>06 Foundations for Inference</t>
-  </si>
-  <si>
     <t>07 Bivariate Inference</t>
   </si>
   <si>
@@ -223,9 +220,6 @@
   </si>
   <si>
     <t>[Poster prep Stage I](project.html)</t>
-  </si>
-  <si>
-    <t>[HW06 Foundations for Inference](hw/06_foundations.html)</t>
   </si>
   <si>
     <t>[Poster prep Stage II](project.html)</t>
@@ -278,14 +272,6 @@
   </si>
   <si>
     <t>[Poster prep Stage IV](project.html)</t>
-  </si>
-  <si>
-    <t>Quantifying Uncertainty  
-Foundations for Inference</t>
-  </si>
-  <si>
-    <t>Interval Estimation   
-Hypothesis testing Foundations</t>
   </si>
   <si>
     <t>Study Design &amp; Causation  
@@ -385,10 +371,6 @@
   </si>
   <si>
     <t>t11_exp_design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[OpenIntro Statistics textbook Ch5](https://leanpub.com/openintro-statistics) or Dr. D's [Math 315 course notes Ch4](https://norcalbiostat.github.io/MATH315/reading/RAD_course_notes_f19.pdf) 
-</t>
   </si>
   <si>
     <t xml:space="preserve">Write down several research questions
@@ -477,9 +459,6 @@
     <t>t05-describing_relationships</t>
   </si>
   <si>
-    <t>t06-probability</t>
-  </si>
-  <si>
     <t>PMA6 Ch 4  
 ASCN Ch 2.4</t>
   </si>
@@ -499,65 +478,82 @@
     <t xml:space="preserve">Create appropriate summary statistics and visualizations for combinations of two measures. </t>
   </si>
   <si>
-    <t>Construct a confidence interval given summary statistics  
-Interpret a confidence interval in context of the problem
-Complete each of the five steps to a quality hypothesis test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identify and distinguish between a parameter and a statistic  
-Calculate a simple probability of exploding.   
-Describe how to generate a sampling distribution using simulation  
-Explain the difference between a probability distribution and a sampling distribution.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Describe the concept of sampling variability.  
+    <t>If all else fails, use "significant at p&gt;.05 level" and hope no one notices. Ref: https://xkcd.com/1478/</t>
+  </si>
+  <si>
+    <t>Describing relationships between two variables</t>
+  </si>
+  <si>
+    <t>Bivariate relationships cont.</t>
+  </si>
+  <si>
+    <t>Labor Day. No Class</t>
+  </si>
+  <si>
+    <t>Correlation &amp; Regression</t>
+  </si>
+  <si>
+    <t>Moderation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stratification  </t>
+  </si>
+  <si>
+    <t>Confounding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple Regression analysis  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model Building  </t>
+  </si>
+  <si>
+    <t>Study Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How did the data come to be? </t>
+  </si>
+  <si>
+    <t>[Study Design](https://hackmd.io/@norcalbiostat/06-study_design)</t>
+  </si>
+  <si>
+    <t>[Introduction to Modern Statistics - Chapter 2](https://openintro-ims.netlify.app/data-design.html)</t>
+  </si>
+  <si>
+    <t>Identify and distinguish between a parameter and a statistic  
+Describe multiple sampling methods
+Identify if a causal statement can be made given a data collection method</t>
+  </si>
+  <si>
+    <t>[What is a sampling distribution](https://youtu.be/xGVzHxFnaiA)
+[Sampling Distributions: Introduction to the concept](https://youtu.be/Zbw-YvELsaM)</t>
+  </si>
+  <si>
+    <t>[Introduction to Modern Statistics - Chapter 13.1-13.3](https://openintro-ims.netlify.app/foundations-mathematical.html)</t>
+  </si>
+  <si>
+    <t>t06-study_design</t>
+  </si>
+  <si>
+    <t>t07-intro_inference</t>
+  </si>
+  <si>
+    <t>Inference with Mathematical Models</t>
+  </si>
+  <si>
+    <t>[Inference with Mathematical models](https://hackmd.io/@norcalbiostat/07-intro_inference)</t>
+  </si>
+  <si>
+    <t>Use the Normal distribution to calculate a probability
+Compare values under two distributions by comparing Zscores
+Describe the concept of sampling variability.  
 Calculate the mean and sd of the sampling distribution based on population parameters  
-Explain the Central Limit Theorem  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">It's okay to say you don't know. </t>
-  </si>
-  <si>
-    <t>If all else fails, use "significant at p&gt;.05 level" and hope no one notices. Ref: https://xkcd.com/1478/</t>
-  </si>
-  <si>
-    <t>Not just for gambling</t>
-  </si>
-  <si>
-    <t>Understanding probability through simulation</t>
-  </si>
-  <si>
-    <t>t07-sampling</t>
-  </si>
-  <si>
-    <t>t08-estimation</t>
-  </si>
-  <si>
-    <t>Describing relationships between two variables</t>
-  </si>
-  <si>
-    <t>Bivariate relationships cont.</t>
-  </si>
-  <si>
-    <t>Labor Day. No Class</t>
-  </si>
-  <si>
-    <t>Correlation &amp; Regression</t>
-  </si>
-  <si>
-    <t>Moderation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stratification  </t>
-  </si>
-  <si>
-    <t>Confounding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiple Regression analysis  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model Building  </t>
+Explain the Central Limit Theorem  
+Construct and Interpret a confidence interval in context of the problem
+Assess a research question using a hypothesis test</t>
+  </si>
+  <si>
+    <t>lec07-intro_inference</t>
   </si>
 </sst>
 </file>
@@ -567,7 +563,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -658,6 +654,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -848,7 +851,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1013,6 +1016,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1444,8 +1450,8 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1460,8 @@
     <col min="3" max="3" width="10.75" style="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.75" style="3" customWidth="1"/>
     <col min="5" max="6" width="19.25" style="3" customWidth="1"/>
-    <col min="7" max="8" width="21" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="21" style="3" customWidth="1"/>
     <col min="9" max="9" width="22" style="3" customWidth="1"/>
     <col min="10" max="10" width="17.625" style="3" customWidth="1"/>
     <col min="11" max="11" width="25.125" style="28" customWidth="1"/>
@@ -1464,40 +1471,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>97</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>101</v>
       </c>
       <c r="I1" s="34" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K1" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="37" t="s">
         <v>95</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1511,31 +1518,31 @@
         <v>43333</v>
       </c>
       <c r="D2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="44" t="s">
+      <c r="G2" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="41" t="s">
+      <c r="J2" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" s="42" t="s">
         <v>96</v>
-      </c>
-      <c r="J2" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" s="42" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="189" x14ac:dyDescent="0.25">
@@ -1546,29 +1553,29 @@
         <v>43333</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J3" s="45"/>
       <c r="K3" s="41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -1580,10 +1587,10 @@
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="54" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
@@ -1603,29 +1610,29 @@
         <v>43340</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I5" s="48" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="41" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1636,29 +1643,29 @@
         <v>43342</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="41" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1673,7 +1680,7 @@
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="51" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="44"/>
@@ -1692,10 +1699,10 @@
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="51" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G8" s="44"/>
       <c r="H8" s="44"/>
@@ -1715,27 +1722,27 @@
         <v>43354</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G9" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="44" t="s">
         <v>124</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="I9" s="44" t="s">
-        <v>129</v>
       </c>
       <c r="J9" s="44"/>
       <c r="K9" s="44"/>
       <c r="L9" s="42" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1756,7 +1763,7 @@
       <c r="J10" s="49"/>
       <c r="K10" s="50"/>
       <c r="L10" s="54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
@@ -1770,27 +1777,27 @@
         <v>43361</v>
       </c>
       <c r="D11" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>143</v>
-      </c>
       <c r="G11" s="41" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="J11" s="44"/>
       <c r="K11" s="44"/>
       <c r="L11" s="42" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1804,7 +1811,7 @@
         <v>43368</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
@@ -1830,10 +1837,10 @@
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="38" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="204.75" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>7</v>
       </c>
@@ -1844,51 +1851,61 @@
         <v>43375</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F14" s="41" t="s">
         <v>150</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H14" s="28"/>
-      <c r="I14" s="28" t="s">
-        <v>111</v>
+      <c r="I14" s="41" t="s">
+        <v>152</v>
       </c>
       <c r="J14" s="28"/>
-      <c r="L14" s="40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="126" x14ac:dyDescent="0.25">
+      <c r="K14" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="L14" s="42"/>
+    </row>
+    <row r="15" spans="1:12" ht="236.25" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>7.2</v>
       </c>
       <c r="C15" s="31">
         <v>43377</v>
       </c>
-      <c r="D15" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
+      <c r="D15" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15" s="41" t="s">
+        <v>159</v>
+      </c>
       <c r="L15" s="40"/>
     </row>
-    <row r="16" spans="1:12" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>8</v>
       </c>
@@ -1898,18 +1915,10 @@
       <c r="C16" s="31">
         <v>43382</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>145</v>
-      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="28"/>
       <c r="J16" s="28"/>
       <c r="L16" s="29"/>
@@ -1922,17 +1931,17 @@
         <v>43384</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
       <c r="J17" s="28"/>
       <c r="L17" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -1947,7 +1956,7 @@
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F18" s="28"/>
     </row>
@@ -1960,7 +1969,7 @@
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
@@ -1980,7 +1989,7 @@
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
@@ -2008,7 +2017,7 @@
       <c r="J21" s="38"/>
       <c r="K21" s="39"/>
       <c r="L21" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2022,17 +2031,17 @@
         <v>43403</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="F22" s="28"/>
       <c r="I22" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2044,7 +2053,7 @@
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="F23" s="28"/>
       <c r="L23" s="29"/>
@@ -2061,7 +2070,7 @@
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
@@ -2071,7 +2080,7 @@
       </c>
       <c r="J24" s="28"/>
       <c r="L24" s="29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2083,7 +2092,7 @@
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -2112,7 +2121,7 @@
       </c>
       <c r="J26" s="28"/>
       <c r="L26" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2123,7 +2132,7 @@
         <v>43419</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>29</v>
@@ -2154,7 +2163,7 @@
       <c r="J28" s="38"/>
       <c r="K28" s="39"/>
       <c r="L28" s="38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2168,10 +2177,10 @@
         <v>43431</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
@@ -2193,11 +2202,11 @@
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F30" s="28"/>
       <c r="L30" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -2208,10 +2217,10 @@
         <v>43440</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
@@ -2235,7 +2244,7 @@
         <v>10</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
@@ -2249,7 +2258,7 @@
         <v>6</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2260,10 +2269,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB861DFA-F44D-408D-9771-0C086E04E7DE}">
-  <dimension ref="A1:V83"/>
+  <dimension ref="A1:V82"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2346,12 +2355,12 @@
         <v>0</v>
       </c>
       <c r="I2" s="8">
-        <f>SUMIF($C$2:$C$74,H2,$D$2:$D$74)</f>
-        <v>100</v>
+        <f>SUMIF($C$2:$C$73,H2,$D$2:$D$73)</f>
+        <v>90</v>
       </c>
       <c r="J2" s="9">
         <f>I2/$I$7</f>
-        <v>0.29411764705882354</v>
+        <v>0.25714285714285712</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>0</v>
@@ -2389,12 +2398,12 @@
         <v>7</v>
       </c>
       <c r="I3" s="6">
-        <f>SUMIF($C$2:$C$74,H3,$D$2:$D$74)</f>
+        <f>SUMIF($C$2:$C$73,H3,$D$2:$D$73)</f>
         <v>60</v>
       </c>
       <c r="J3" s="12">
         <f>I3/$I$7</f>
-        <v>0.17647058823529413</v>
+        <v>0.17142857142857143</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>7</v>
@@ -2420,7 +2429,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -2432,12 +2441,12 @@
         <v>4</v>
       </c>
       <c r="I4" s="15">
-        <f>SUMIF($C$2:$C$74,H4,$D$2:$D$74)</f>
+        <f>SUMIF($C$2:$C$73,H4,$D$2:$D$73)</f>
         <v>50</v>
       </c>
       <c r="J4" s="16">
         <f>I4/$I$7</f>
-        <v>0.14705882352941177</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>4</v>
@@ -2475,12 +2484,12 @@
         <v>8</v>
       </c>
       <c r="I5" s="21">
-        <f>SUMIF($C$2:$C$74,H5,$D$2:$D$74)</f>
-        <v>30</v>
+        <f>SUMIF($C$2:$C$73,H5,$D$2:$D$73)</f>
+        <v>50</v>
       </c>
       <c r="J5" s="22">
         <f>I5/$I$7</f>
-        <v>8.8235294117647065E-2</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="P5" s="20" t="s">
         <v>8</v>
@@ -2518,12 +2527,12 @@
         <v>5</v>
       </c>
       <c r="I6" s="13">
-        <f>SUMIF($C$2:$C$74,H6,$D$2:$D$74)</f>
+        <f>SUMIF($C$2:$C$73,H6,$D$2:$D$73)</f>
         <v>100</v>
       </c>
       <c r="J6" s="18">
         <f>I6/$I$7</f>
-        <v>0.29411764705882354</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="P6" s="17" t="s">
         <v>5</v>
@@ -2554,7 +2563,7 @@
       </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="Q7" s="19">
         <f>SUM(Q2:Q6)</f>
@@ -2595,7 +2604,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>7</v>
@@ -2634,162 +2643,163 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>6.2</v>
+        <v>7</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="10">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="13">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
+        <v>7.1</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="13">
-        <v>20</v>
+      <c r="D14" s="26">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>7.1</v>
+        <v>7.3</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="26">
-        <v>6</v>
+        <v>43</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>7.3</v>
+        <v>8</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="10">
-        <v>10</v>
-      </c>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6">
+        <v>3</v>
+      </c>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>8</v>
+        <v>8.4</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="6">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="13">
+        <v>20</v>
       </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>8.4</v>
+        <v>8.5</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="13">
-        <v>20</v>
+        <v>54</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="26">
+        <v>6</v>
       </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="26">
-        <v>6</v>
+        <v>45</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10">
+        <v>10</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>8.6</v>
+        <v>9</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="10">
-        <v>10</v>
+      <c r="C20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6">
+        <v>3</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>9</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="6">
-        <v>3</v>
+        <v>48</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10">
+        <v>10</v>
       </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>9.1999999999999993</v>
+        <v>10</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="10">
-        <v>10</v>
+        <v>47</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="6">
+        <v>3</v>
       </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
         <v>10</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="6">
-        <v>3</v>
       </c>
       <c r="I23" s="3"/>
     </row>
@@ -2798,58 +2808,58 @@
         <v>10.199999999999999</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="10">
+        <v>24</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="13">
         <v>10</v>
       </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>10.199999999999999</v>
+        <v>10.5</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="13">
-        <v>10</v>
+        <v>55</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="26">
+        <v>6</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>10.5</v>
+        <v>10.6</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="26">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="13">
+        <v>10</v>
       </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>10.6</v>
+        <v>11</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="13">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="6">
+        <v>3</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2858,91 +2868,87 @@
         <v>11</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="6">
-        <v>3</v>
+      <c r="D28" s="26">
+        <v>6</v>
       </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>11</v>
+        <v>11.2</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="26">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="13">
+        <v>20</v>
       </c>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>11.2</v>
+        <v>12</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="13">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="26">
+        <v>6</v>
       </c>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>12</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="26">
+        <v>12.1</v>
+      </c>
+      <c r="B31" s="24" t="s">
         <v>6</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="15">
+        <v>50</v>
       </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>12.1</v>
+        <v>0</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="15">
+        <v>66</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="21">
         <v>50</v>
       </c>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>0</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="21">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="24"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="24"/>
       <c r="F37" s="5"/>
       <c r="G37" s="3"/>
@@ -2953,7 +2959,7 @@
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="24"/>
       <c r="F38" s="5"/>
       <c r="G38" s="3"/>
@@ -2964,7 +2970,7 @@
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
     </row>
-    <row r="39" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="24"/>
       <c r="F39" s="5"/>
       <c r="G39" s="3"/>
@@ -2975,7 +2981,7 @@
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
     </row>
-    <row r="40" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="24"/>
       <c r="F40" s="5"/>
       <c r="G40" s="3"/>
@@ -2986,7 +2992,7 @@
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
     </row>
-    <row r="41" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="24"/>
       <c r="F41" s="5"/>
       <c r="G41" s="3"/>
@@ -2997,7 +3003,7 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="24"/>
       <c r="F42" s="5"/>
       <c r="G42" s="3"/>
@@ -3008,7 +3014,7 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="24"/>
       <c r="F43" s="5"/>
       <c r="G43" s="3"/>
@@ -3019,7 +3025,7 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="24"/>
       <c r="F44" s="5"/>
       <c r="G44" s="3"/>
@@ -3030,7 +3036,7 @@
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="24"/>
       <c r="F45" s="5"/>
       <c r="G45" s="3"/>
@@ -3041,7 +3047,7 @@
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="24"/>
       <c r="F46" s="5"/>
       <c r="G46" s="3"/>
@@ -3052,7 +3058,7 @@
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="24"/>
       <c r="F47" s="5"/>
       <c r="G47" s="3"/>
@@ -3063,7 +3069,7 @@
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="24"/>
       <c r="F48" s="5"/>
       <c r="G48" s="3"/>
@@ -3107,24 +3113,24 @@
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
     </row>
-    <row r="52" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="24"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
+    <row r="68" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="24"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
     </row>
     <row r="69" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="24"/>
       <c r="F69" s="5"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
@@ -3136,6 +3142,8 @@
       <c r="F70" s="5"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
@@ -3238,8 +3246,6 @@
       <c r="F78" s="5"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
       <c r="L78" s="3"/>
       <c r="M78" s="3"/>
       <c r="N78" s="3"/>
@@ -3290,20 +3296,9 @@
       <c r="O82" s="3"/>
       <c r="P82" s="3"/>
     </row>
-    <row r="83" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="24"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-      <c r="L83" s="3"/>
-      <c r="M83" s="3"/>
-      <c r="N83" s="3"/>
-      <c r="O83" s="3"/>
-      <c r="P83" s="3"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D96">
-    <sortCondition ref="A2:A96"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D95">
+    <sortCondition ref="A2:A95"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
use hack to get hyperlinks to work on schedule table
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D600D607-3A56-413B-AF06-4DE9C2005096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115BC753-F3E0-4AC1-BE60-E3C09E2C5839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30300" yWindow="330" windowWidth="22740" windowHeight="15420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="164">
   <si>
     <t>Assignment</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>[Poster prep Stage II](project.html)</t>
-  </si>
-  <si>
-    <t>[HW07 Bivariate Inference](hw/07_bivariate_inference.html)</t>
   </si>
   <si>
     <t>[HW10 GLM &amp; Categorical](hw/10_GLM_catpreds.html)</t>
@@ -532,29 +529,40 @@
     <t>t07-intro_inference</t>
   </si>
   <si>
-    <t>Inference with Mathematical Models</t>
-  </si>
-  <si>
     <t>[Inference with Mathematical models](https://hackmd.io/@norcalbiostat/07-intro_inference)</t>
   </si>
   <si>
+    <t>lec07-intro_inference</t>
+  </si>
+  <si>
+    <t>[IMS - Chapter 13.1-13.3](https://openintro-ims.netlify.app/foundations-mathematical.html)
+and [IMS Chapter 11-11.1](https://openintro-ims.netlify.app/foundations-randomization.html)</t>
+  </si>
+  <si>
+    <t>[IMS - Chapter 2](https://openintro-ims.netlify.app/data-design.html)</t>
+  </si>
+  <si>
+    <t>Explain how to test a hypothsis using randomization
+Assess a research question using a hypothesis test</t>
+  </si>
+  <si>
     <t>Use the Normal distribution to calculate a probability
-Compare values under two distributions by comparing Zscores
 Describe the concept of sampling variability.  
 Calculate the mean and sd of the sampling distribution based on population parameters  
 Explain the Central Limit Theorem  
 Construct and Interpret a confidence interval in context of the problem
-Assess a research question using a hypothesis test</t>
-  </si>
-  <si>
-    <t>lec07-intro_inference</t>
-  </si>
-  <si>
-    <t>[IMS - Chapter 13.1-13.3](https://openintro-ims.netlify.app/foundations-mathematical.html)
-and [IMS Chapter 11-11.1](https://openintro-ims.netlify.app/foundations-randomization.html)</t>
-  </si>
-  <si>
-    <t>[IMS - Chapter 2](https://openintro-ims.netlify.app/data-design.html)</t>
+Use a confidence interval to make an inferential hypothesis statement</t>
+  </si>
+  <si>
+    <t>[HW06 Bivariate Inference](hw/06_bivariate_inference.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundations for Inference
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundations for Inference cont.
+</t>
   </si>
 </sst>
 </file>
@@ -1440,9 +1448,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1451,7 +1459,7 @@
     <col min="3" max="3" width="10.75" style="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.75" style="3" customWidth="1"/>
     <col min="5" max="6" width="19.25" style="3" customWidth="1"/>
-    <col min="7" max="7" width="29.875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="40" style="3" customWidth="1"/>
     <col min="8" max="8" width="21" style="3" customWidth="1"/>
     <col min="9" max="9" width="22" style="3" customWidth="1"/>
     <col min="10" max="10" width="17.625" style="3" customWidth="1"/>
@@ -1462,28 +1470,28 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>68</v>
-      </c>
       <c r="D1" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>87</v>
-      </c>
       <c r="G1" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I1" s="34" t="s">
         <v>31</v>
@@ -1492,10 +1500,10 @@
         <v>57</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1509,34 +1517,34 @@
         <v>43333</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J2" s="45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K2" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L2" s="42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="141.75" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
       <c r="B3" s="27">
         <v>1.2</v>
       </c>
@@ -1544,29 +1552,29 @@
         <v>43333</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J3" s="45"/>
       <c r="K3" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -1578,10 +1586,10 @@
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
@@ -1601,29 +1609,29 @@
         <v>43340</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" s="48" t="s">
         <v>109</v>
-      </c>
-      <c r="F5" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="H5" s="41" t="s">
-        <v>126</v>
-      </c>
-      <c r="I5" s="48" t="s">
-        <v>110</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1634,29 +1642,29 @@
         <v>43342</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1671,7 +1679,7 @@
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="44"/>
@@ -1690,10 +1698,10 @@
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="41" t="s">
         <v>114</v>
-      </c>
-      <c r="F8" s="41" t="s">
-        <v>115</v>
       </c>
       <c r="G8" s="44"/>
       <c r="H8" s="44"/>
@@ -1713,27 +1721,27 @@
         <v>43354</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="G9" s="41" t="s">
-        <v>119</v>
-      </c>
       <c r="H9" s="41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I9" s="44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J9" s="44"/>
       <c r="K9" s="44"/>
       <c r="L9" s="42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1768,27 +1776,27 @@
         <v>43361</v>
       </c>
       <c r="D11" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" s="44" t="s">
         <v>132</v>
-      </c>
-      <c r="E11" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="G11" s="41" t="s">
-        <v>138</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="I11" s="44" t="s">
-        <v>133</v>
       </c>
       <c r="J11" s="44"/>
       <c r="K11" s="44"/>
       <c r="L11" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1802,7 +1810,7 @@
         <v>43368</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
@@ -1831,7 +1839,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>7</v>
       </c>
@@ -1842,28 +1850,28 @@
         <v>43375</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E14" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="F14" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="41" t="s">
-        <v>150</v>
-      </c>
       <c r="G14" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="41" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L14" s="42"/>
     </row>
-    <row r="15" spans="1:12" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>7.2</v>
       </c>
@@ -1871,32 +1879,32 @@
         <v>43377</v>
       </c>
       <c r="D15" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="K15" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="E15" s="41" t="s">
-        <v>156</v>
-      </c>
-      <c r="F15" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>159</v>
-      </c>
-      <c r="I15" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="J15" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="K15" s="41" t="s">
-        <v>157</v>
-      </c>
       <c r="L15" s="40"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>8</v>
       </c>
@@ -1907,9 +1915,13 @@
         <v>43382</v>
       </c>
       <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
+      <c r="E16" s="41" t="s">
+        <v>163</v>
+      </c>
       <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
+      <c r="G16" s="41" t="s">
+        <v>160</v>
+      </c>
       <c r="H16" s="28"/>
       <c r="J16" s="28"/>
       <c r="L16" s="29"/>
@@ -1921,18 +1933,17 @@
       <c r="C17" s="31">
         <v>43384</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>102</v>
-      </c>
       <c r="E17" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
+      <c r="G17" s="28" t="s">
+        <v>101</v>
+      </c>
       <c r="H17" s="28"/>
       <c r="J17" s="28"/>
       <c r="L17" s="3" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -1947,7 +1958,7 @@
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F18" s="28"/>
     </row>
@@ -1960,7 +1971,7 @@
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
@@ -1980,7 +1991,7 @@
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
@@ -2008,7 +2019,7 @@
       <c r="J21" s="38"/>
       <c r="K21" s="39"/>
       <c r="L21" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2021,18 +2032,18 @@
       <c r="C22" s="31">
         <v>43403</v>
       </c>
-      <c r="D22" s="28" t="s">
-        <v>103</v>
-      </c>
       <c r="E22" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F22" s="28"/>
+      <c r="G22" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="I22" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2044,7 +2055,7 @@
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F23" s="28"/>
       <c r="L23" s="29"/>
@@ -2061,7 +2072,7 @@
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
@@ -2071,7 +2082,7 @@
       </c>
       <c r="J24" s="28"/>
       <c r="L24" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2083,7 +2094,7 @@
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -2112,7 +2123,7 @@
       </c>
       <c r="J26" s="28"/>
       <c r="L26" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2122,13 +2133,12 @@
       <c r="C27" s="31">
         <v>43419</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="E27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="28"/>
+      <c r="G27" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="H27" s="28"/>
       <c r="I27" s="28" t="s">
         <v>34</v>
@@ -2154,7 +2164,7 @@
       <c r="J28" s="38"/>
       <c r="K28" s="39"/>
       <c r="L28" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2167,14 +2177,13 @@
       <c r="C29" s="31">
         <v>43431</v>
       </c>
-      <c r="D29" s="28" t="s">
-        <v>105</v>
-      </c>
       <c r="E29" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
+      <c r="G29" s="28" t="s">
+        <v>104</v>
+      </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28" t="s">
         <v>37</v>
@@ -2191,13 +2200,13 @@
       <c r="C30" s="31">
         <v>43438</v>
       </c>
-      <c r="D30" s="28"/>
       <c r="E30" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
       <c r="L30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -2207,14 +2216,13 @@
       <c r="C31" s="31">
         <v>43440</v>
       </c>
-      <c r="D31" s="28" t="s">
-        <v>106</v>
-      </c>
       <c r="E31" s="47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
+      <c r="G31" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28" t="s">
         <v>39</v>
@@ -2249,7 +2257,7 @@
         <v>6</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2919,7 +2927,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add data viz start bivariate analysis
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115BC753-F3E0-4AC1-BE60-E3C09E2C5839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477276CF-0D89-4376-A40E-57D96C80AABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30300" yWindow="330" windowWidth="22740" windowHeight="15420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="172">
   <si>
     <t>Assignment</t>
   </si>
@@ -174,9 +174,6 @@
     <t>05 PR</t>
   </si>
   <si>
-    <t>07 Bivariate Inference</t>
-  </si>
-  <si>
     <t>07 PR</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>T-tests for difference in means</t>
   </si>
   <si>
     <t>Preparing data for analysis</t>
@@ -353,9 +347,6 @@
   </si>
   <si>
     <t>Project Stage 1: Choosing your topic</t>
-  </si>
-  <si>
-    <t>t07_biv_inf</t>
   </si>
   <si>
     <t>t08_mv_inf</t>
@@ -481,9 +472,6 @@
     <t>Describing relationships between two variables</t>
   </si>
   <si>
-    <t>Bivariate relationships cont.</t>
-  </si>
-  <si>
     <t>Labor Day. No Class</t>
   </si>
   <si>
@@ -542,27 +530,66 @@
     <t>[IMS - Chapter 2](https://openintro-ims.netlify.app/data-design.html)</t>
   </si>
   <si>
+    <t xml:space="preserve">Foundations for Inference
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundations for Inference cont.
+</t>
+  </si>
+  <si>
+    <t>t08_bivariate_modeling</t>
+  </si>
+  <si>
+    <t>Modeling Bivariate relationships</t>
+  </si>
+  <si>
+    <t>lec06-data_viz_bestpractice</t>
+  </si>
+  <si>
+    <t>Best practices in Data Visualization</t>
+  </si>
+  <si>
+    <t>Just because you can add it to a graph, doesn't mean you should.</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 4.6</t>
+  </si>
+  <si>
+    <t>[Choosing appropriate analysis](https://hackmd.io/@norcalbiostat/08-choosing-analysis)</t>
+  </si>
+  <si>
+    <t>Inference with Mathematical Models</t>
+  </si>
+  <si>
+    <t>lec08-bivariate_modeling</t>
+  </si>
+  <si>
+    <t>[HW06 Bivariate Modeling](hw/06_biv_modeling.html)</t>
+  </si>
+  <si>
+    <t>06 Bivariate Inference</t>
+  </si>
+  <si>
+    <t>Choosing appropriate analysis, 
+T-tests for difference in means</t>
+  </si>
+  <si>
+    <t>Identify the most appropriate analysis for a given research topic. 
+Fully conduct the following statistical analyses: Two sample T-Test of means, ANOVA,  Chi-squared test of Association, Correlation, Simple linear Regression</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 6</t>
+  </si>
+  <si>
     <t>Explain how to test a hypothsis using randomization
-Assess a research question using a hypothesis test</t>
-  </si>
-  <si>
-    <t>Use the Normal distribution to calculate a probability
-Describe the concept of sampling variability.  
-Calculate the mean and sd of the sampling distribution based on population parameters  
-Explain the Central Limit Theorem  
+Assess a research question using a hypothesis test
+Use the Normal distribution to calculate a probability
+Describe the concept of sampling variability
+Calculate the mean and sd of the sampling distribution based on population parameters
+Explain the Central Limit Theorem
 Construct and Interpret a confidence interval in context of the problem
 Use a confidence interval to make an inferential hypothesis statement</t>
-  </si>
-  <si>
-    <t>[HW06 Bivariate Inference](hw/06_bivariate_inference.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foundations for Inference
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Foundations for Inference cont.
-</t>
   </si>
 </sst>
 </file>
@@ -572,7 +599,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -663,6 +690,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -853,7 +887,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -996,9 +1030,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1019,6 +1050,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -1448,15 +1485,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.875" style="4"/>
-    <col min="3" max="3" width="10.75" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="30" customWidth="1"/>
     <col min="4" max="4" width="13.75" style="3" customWidth="1"/>
     <col min="5" max="6" width="19.25" style="3" customWidth="1"/>
     <col min="7" max="7" width="40" style="3" customWidth="1"/>
@@ -1470,40 +1507,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B1" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" s="34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E1" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="34" t="s">
-        <v>86</v>
-      </c>
       <c r="G1" s="34" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I1" s="34" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1517,31 +1554,31 @@
         <v>43333</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="I2" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="K2" s="41" t="s">
-        <v>82</v>
-      </c>
       <c r="L2" s="42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
@@ -1552,51 +1589,51 @@
         <v>43333</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="44" t="s">
-        <v>99</v>
+        <v>119</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>97</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J3" s="45"/>
       <c r="K3" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="52">
+      <c r="B4" s="51">
         <v>1.3</v>
       </c>
-      <c r="C4" s="53">
+      <c r="C4" s="52">
         <v>43335</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="48"/>
     </row>
     <row r="5" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -1609,29 +1646,29 @@
         <v>43340</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G5" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="I5" s="56" t="s">
         <v>106</v>
-      </c>
-      <c r="H5" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="I5" s="48" t="s">
-        <v>109</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1642,29 +1679,29 @@
         <v>43342</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="I6" s="44" t="s">
-        <v>110</v>
+        <v>121</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>107</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1678,13 +1715,13 @@
         <v>43347</v>
       </c>
       <c r="D7" s="45"/>
-      <c r="E7" s="51" t="s">
-        <v>141</v>
+      <c r="E7" s="50" t="s">
+        <v>137</v>
       </c>
       <c r="F7" s="41"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
       <c r="J7" s="44"/>
       <c r="K7" s="44"/>
       <c r="L7" s="46"/>
@@ -1697,15 +1734,15 @@
         <v>43349</v>
       </c>
       <c r="D8" s="45"/>
-      <c r="E8" s="51" t="s">
-        <v>113</v>
+      <c r="E8" s="50" t="s">
+        <v>110</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
+        <v>111</v>
+      </c>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="44"/>
       <c r="K8" s="44"/>
       <c r="L8" s="46"/>
@@ -1721,27 +1758,27 @@
         <v>43354</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G9" s="41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H9" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="I9" s="44" t="s">
-        <v>123</v>
+        <v>131</v>
+      </c>
+      <c r="I9" s="41" t="s">
+        <v>120</v>
       </c>
       <c r="J9" s="44"/>
       <c r="K9" s="44"/>
       <c r="L9" s="42" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1752,17 +1789,17 @@
         <v>43356</v>
       </c>
       <c r="D10" s="38"/>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="54" t="s">
-        <v>58</v>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="53" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1776,30 +1813,30 @@
         <v>43361</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="I11" s="44" t="s">
-        <v>132</v>
+        <v>130</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>129</v>
       </c>
       <c r="J11" s="44"/>
       <c r="K11" s="44"/>
       <c r="L11" s="42" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -1809,12 +1846,19 @@
       <c r="C12" s="31">
         <v>43368</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
+      <c r="E12" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>162</v>
+      </c>
       <c r="J12" s="28"/>
       <c r="L12" s="29"/>
     </row>
@@ -1836,7 +1880,7 @@
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
@@ -1850,28 +1894,28 @@
         <v>43375</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="41" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="41" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L14" s="42"/>
     </row>
-    <row r="15" spans="1:12" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="220.5" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>7.2</v>
       </c>
@@ -1879,32 +1923,32 @@
         <v>43377</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K15" s="41" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="L15" s="40"/>
     </row>
-    <row r="16" spans="1:12" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>8</v>
       </c>
@@ -1916,34 +1960,47 @@
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="41" t="s">
-        <v>160</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" s="41"/>
       <c r="H16" s="28"/>
       <c r="J16" s="28"/>
       <c r="L16" s="29"/>
     </row>
-    <row r="17" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B17" s="27">
         <v>8.1999999999999993</v>
       </c>
       <c r="C17" s="31">
         <v>43384</v>
       </c>
-      <c r="E17" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="H17" s="28"/>
+      <c r="D17" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="H17" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="J17" s="28"/>
-      <c r="L17" s="3" t="s">
-        <v>161</v>
+      <c r="K17" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="L17" s="50" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -1957,10 +2014,10 @@
         <v>43389</v>
       </c>
       <c r="D18" s="28"/>
-      <c r="E18" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B19" s="27">
@@ -1970,10 +2027,10 @@
         <v>43391</v>
       </c>
       <c r="D19" s="28"/>
-      <c r="E19" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28" t="s">
+        <v>69</v>
+      </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
@@ -1990,10 +2047,10 @@
         <v>43396</v>
       </c>
       <c r="D20" s="28"/>
-      <c r="E20" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="F20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28" t="s">
+        <v>138</v>
+      </c>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28" t="s">
@@ -2019,7 +2076,7 @@
       <c r="J21" s="38"/>
       <c r="K21" s="39"/>
       <c r="L21" s="38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2033,17 +2090,17 @@
         <v>43403</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>35</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2055,7 +2112,7 @@
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F23" s="28"/>
       <c r="L23" s="29"/>
@@ -2072,7 +2129,7 @@
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
@@ -2082,7 +2139,7 @@
       </c>
       <c r="J24" s="28"/>
       <c r="L24" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2094,7 +2151,7 @@
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -2123,7 +2180,7 @@
       </c>
       <c r="J26" s="28"/>
       <c r="L26" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2137,7 +2194,7 @@
         <v>29</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="28" t="s">
@@ -2164,7 +2221,7 @@
       <c r="J28" s="38"/>
       <c r="K28" s="39"/>
       <c r="L28" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2178,11 +2235,11 @@
         <v>43431</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="28" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28" t="s">
@@ -2201,12 +2258,12 @@
         <v>43438</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
       <c r="L30" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -2217,11 +2274,11 @@
         <v>43440</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28" t="s">
@@ -2243,7 +2300,7 @@
         <v>10</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
@@ -2257,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2271,7 +2328,7 @@
   <dimension ref="A1:V82"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2359,7 +2416,7 @@
       </c>
       <c r="J2" s="9">
         <f>I2/$I$7</f>
-        <v>0.25714285714285712</v>
+        <v>0.26470588235294118</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>0</v>
@@ -2398,11 +2455,11 @@
       </c>
       <c r="I3" s="6">
         <f>SUMIF($C$2:$C$73,H3,$D$2:$D$73)</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J3" s="12">
         <f>I3/$I$7</f>
-        <v>0.17142857142857143</v>
+        <v>0.19117647058823528</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>7</v>
@@ -2428,7 +2485,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -2445,7 +2502,7 @@
       </c>
       <c r="J4" s="16">
         <f>I4/$I$7</f>
-        <v>0.14285714285714285</v>
+        <v>0.14705882352941177</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>4</v>
@@ -2484,11 +2541,11 @@
       </c>
       <c r="I5" s="21">
         <f>SUMIF($C$2:$C$73,H5,$D$2:$D$73)</f>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="J5" s="22">
         <f>I5/$I$7</f>
-        <v>0.14285714285714285</v>
+        <v>0.10294117647058823</v>
       </c>
       <c r="P5" s="20" t="s">
         <v>8</v>
@@ -2531,7 +2588,7 @@
       </c>
       <c r="J6" s="18">
         <f>I6/$I$7</f>
-        <v>0.2857142857142857</v>
+        <v>0.29411764705882354</v>
       </c>
       <c r="P6" s="17" t="s">
         <v>5</v>
@@ -2562,7 +2619,7 @@
       </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="Q7" s="19">
         <f>SUM(Q2:Q6)</f>
@@ -2603,7 +2660,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>7</v>
@@ -2637,12 +2694,12 @@
         <v>7</v>
       </c>
       <c r="D12" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>7</v>
+        <v>5.2</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>22</v>
@@ -2656,10 +2713,10 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>7.1</v>
+        <v>5.3</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>7</v>
@@ -2670,10 +2727,10 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <v>7.3</v>
+        <v>8</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>43</v>
+        <v>167</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>0</v>
@@ -2684,22 +2741,22 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>8</v>
+        <v>8.1</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>8.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>23</v>
@@ -2714,10 +2771,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <v>8.5</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>7</v>
@@ -2728,11 +2785,8 @@
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>8.6</v>
-      </c>
       <c r="B19" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>0</v>
@@ -2743,11 +2797,8 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>9</v>
-      </c>
       <c r="B20" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>7</v>
@@ -2758,11 +2809,8 @@
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>9.1999999999999993</v>
-      </c>
       <c r="B21" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>0</v>
@@ -2773,11 +2821,8 @@
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>10</v>
-      </c>
       <c r="B22" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>7</v>
@@ -2788,11 +2833,8 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>10.199999999999999</v>
-      </c>
       <c r="B23" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>0</v>
@@ -2803,9 +2845,6 @@
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>10.199999999999999</v>
-      </c>
       <c r="B24" s="25" t="s">
         <v>24</v>
       </c>
@@ -2818,11 +2857,8 @@
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>10.5</v>
-      </c>
       <c r="B25" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>7</v>
@@ -2833,9 +2869,6 @@
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>10.6</v>
-      </c>
       <c r="B26" s="25" t="s">
         <v>16</v>
       </c>
@@ -2848,11 +2881,8 @@
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>11</v>
-      </c>
       <c r="B27" s="25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>7</v>
@@ -2863,9 +2893,6 @@
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>11</v>
-      </c>
       <c r="B28" s="25" t="s">
         <v>17</v>
       </c>
@@ -2878,9 +2905,6 @@
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>11.2</v>
-      </c>
       <c r="B29" s="25" t="s">
         <v>18</v>
       </c>
@@ -2893,9 +2917,6 @@
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>12</v>
-      </c>
       <c r="B30" s="25" t="s">
         <v>19</v>
       </c>
@@ -2908,9 +2929,6 @@
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>12.1</v>
-      </c>
       <c r="B31" s="24" t="s">
         <v>6</v>
       </c>
@@ -2927,13 +2945,13 @@
         <v>0</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="21">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
push changes to index and project
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477276CF-0D89-4376-A40E-57D96C80AABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DA29F5-C19B-4574-BDEA-B37B2C883991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="172">
   <si>
     <t>Assignment</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Quiz</t>
   </si>
   <si>
-    <t>Topic</t>
-  </si>
-  <si>
     <t>Poster Presentation</t>
   </si>
   <si>
@@ -103,28 +100,7 @@
     <t>01 Data Structure and Entry</t>
   </si>
   <si>
-    <t>Poster prep I: Intro to RQ</t>
-  </si>
-  <si>
-    <t>Poster prep II: EDA</t>
-  </si>
-  <si>
-    <t>Poster prep III: Bivariate Analysis</t>
-  </si>
-  <si>
-    <t>Poster prep IV: Multivariate Analysis</t>
-  </si>
-  <si>
     <t>04 Univariate Graphics</t>
-  </si>
-  <si>
-    <t>Project Stage I: Setting up the story</t>
-  </si>
-  <si>
-    <t>Project Stage II: Exploratory Data Analysis</t>
-  </si>
-  <si>
-    <t>Project Stage III: Bivariate Inference</t>
   </si>
   <si>
     <t>Logistic Regression analysis</t>
@@ -177,61 +153,22 @@
     <t>07 PR</t>
   </si>
   <si>
-    <t>08 Moderation</t>
-  </si>
-  <si>
     <t>08 PR</t>
   </si>
   <si>
     <t>09 PR</t>
   </si>
   <si>
-    <t>09 Multiple Regression</t>
-  </si>
-  <si>
-    <t>10 GLM and Categorical Predictors</t>
-  </si>
-  <si>
-    <t>10 PR</t>
-  </si>
-  <si>
     <t>02 PR</t>
   </si>
   <si>
-    <t>PP I: PR</t>
-  </si>
-  <si>
-    <t>PP II: PR</t>
-  </si>
-  <si>
-    <t>PP III: PR</t>
-  </si>
-  <si>
-    <t>PP IV: PR</t>
-  </si>
-  <si>
     <t xml:space="preserve">Monday 6pm-8pm. I will work to get this changed. </t>
   </si>
   <si>
     <t>Video</t>
   </si>
   <si>
-    <t>[Poster prep Stage I](project.html)</t>
-  </si>
-  <si>
-    <t>[Poster prep Stage II](project.html)</t>
-  </si>
-  <si>
-    <t>[HW10 GLM &amp; Categorical](hw/10_GLM_catpreds.html)</t>
-  </si>
-  <si>
     <t>Take home final exam</t>
-  </si>
-  <si>
-    <t>[HW09 Multiple Regression](hw/09_MLR_confounding.html)</t>
-  </si>
-  <si>
-    <t>[HW 08 Moderation](hw/08_moderation.html)</t>
   </si>
   <si>
     <t>Poster*</t>
@@ -263,10 +200,6 @@
   </si>
   <si>
     <t>[Poster prep Stage IV](project.html)</t>
-  </si>
-  <si>
-    <t>Study Design &amp; Causation  
-What to watch out for</t>
   </si>
   <si>
     <t>Welcome Aboard!</t>
@@ -590,6 +523,72 @@
 Explain the Central Limit Theorem
 Construct and Interpret a confidence interval in context of the problem
 Use a confidence interval to make an inferential hypothesis statement</t>
+  </si>
+  <si>
+    <t>[HW08 Multiple Regression](hw/09_MLR_confounding.html)</t>
+  </si>
+  <si>
+    <t>[HW9 GLM &amp; Categorical](hw/10_GLM_catpreds.html)</t>
+  </si>
+  <si>
+    <t>Poster prep Stage 3: EDA</t>
+  </si>
+  <si>
+    <t>Poster prep Stage 4: Bivariate Analysis</t>
+  </si>
+  <si>
+    <t>Poster prep Stage 5: Multivariate Analysis</t>
+  </si>
+  <si>
+    <t>[HW 07 Moderation and Stratification](hw/07_mod_strat.html)</t>
+  </si>
+  <si>
+    <t>Poster prep Stage 2: Intro to RQ &amp; Variables</t>
+  </si>
+  <si>
+    <t>06 PR</t>
+  </si>
+  <si>
+    <t>PPS2: PR</t>
+  </si>
+  <si>
+    <t>PPS3: PR</t>
+  </si>
+  <si>
+    <t>PPS4: PR</t>
+  </si>
+  <si>
+    <t>07 Moderation &amp; Stratification</t>
+  </si>
+  <si>
+    <t>08 Multiple Regression</t>
+  </si>
+  <si>
+    <t>PPS5: PR</t>
+  </si>
+  <si>
+    <t>09 GLM and Categorical Predictors</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>[Poster prep Stage 2](project.html)</t>
+  </si>
+  <si>
+    <t>Project Stage 3: Exploratory Data Analysis</t>
+  </si>
+  <si>
+    <t>[Poster prep Stage 3](project.html)</t>
+  </si>
+  <si>
+    <t>Project Stage 2: Introduce your research question and variables of interest</t>
+  </si>
+  <si>
+    <t>Project Stage 4: Bivariate Inference</t>
+  </si>
+  <si>
+    <t>Other types of models</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1485,8 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1507,40 +1506,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C1" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>88</v>
-      </c>
       <c r="L1" s="37" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1554,31 +1553,31 @@
         <v>43333</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="J2" s="45" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="K2" s="41" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="L2" s="42" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
@@ -1589,29 +1588,29 @@
         <v>43333</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="J3" s="45"/>
       <c r="K3" s="41" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -1623,10 +1622,10 @@
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="53" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
@@ -1646,29 +1645,29 @@
         <v>43340</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="I5" s="56" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="41" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1679,29 +1678,29 @@
         <v>43342</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="I6" s="41" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="41" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1716,7 +1715,7 @@
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="50" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="41"/>
@@ -1735,10 +1734,10 @@
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="50" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="G8" s="41"/>
       <c r="H8" s="41"/>
@@ -1758,27 +1757,27 @@
         <v>43354</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="G9" s="41" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="H9" s="41" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="I9" s="41" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="J9" s="44"/>
       <c r="K9" s="44"/>
       <c r="L9" s="42" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1790,7 +1789,7 @@
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="53" t="s">
-        <v>26</v>
+        <v>169</v>
       </c>
       <c r="F10" s="53"/>
       <c r="G10" s="53"/>
@@ -1799,7 +1798,7 @@
       <c r="J10" s="48"/>
       <c r="K10" s="49"/>
       <c r="L10" s="53" t="s">
-        <v>57</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1813,27 +1812,27 @@
         <v>43361</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="I11" s="41" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="J11" s="44"/>
       <c r="K11" s="44"/>
       <c r="L11" s="42" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1847,17 +1846,17 @@
         <v>43368</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="41" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="J12" s="28"/>
       <c r="L12" s="29"/>
@@ -1871,7 +1870,7 @@
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38" t="s">
-        <v>27</v>
+        <v>167</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
@@ -1880,7 +1879,7 @@
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="38" t="s">
-        <v>58</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
@@ -1894,24 +1893,24 @@
         <v>43375</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="41" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="41" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="L14" s="42"/>
     </row>
@@ -1923,28 +1922,28 @@
         <v>43377</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="K15" s="41" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="L15" s="40"/>
     </row>
@@ -1960,10 +1959,10 @@
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="41" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="28"/>
@@ -1978,29 +1977,29 @@
         <v>43384</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="H17" s="55" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="41" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="L17" s="50" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -2016,7 +2015,7 @@
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2029,7 +2028,7 @@
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -2049,12 +2048,12 @@
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="J20" s="28"/>
     </row>
@@ -2067,7 +2066,7 @@
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38" t="s">
-        <v>28</v>
+        <v>170</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
@@ -2076,7 +2075,7 @@
       <c r="J21" s="38"/>
       <c r="K21" s="39"/>
       <c r="L21" s="38" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2090,17 +2089,17 @@
         <v>43403</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2112,7 +2111,7 @@
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="F23" s="28"/>
       <c r="L23" s="29"/>
@@ -2129,17 +2128,17 @@
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
       <c r="I24" s="28" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="J24" s="28"/>
       <c r="L24" s="29" t="s">
-        <v>61</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2151,7 +2150,7 @@
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -2171,16 +2170,16 @@
         <v>43417</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J26" s="28"/>
       <c r="L26" s="29" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2191,14 +2190,14 @@
         <v>43419</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="28" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J27" s="28"/>
       <c r="L27" s="29"/>
@@ -2212,7 +2211,7 @@
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
@@ -2221,7 +2220,7 @@
       <c r="J28" s="38"/>
       <c r="K28" s="39"/>
       <c r="L28" s="38" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2235,15 +2234,15 @@
         <v>43431</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="28" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J29" s="28"/>
     </row>
@@ -2258,15 +2257,15 @@
         <v>43438</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
       <c r="L30" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="27">
         <v>15.2</v>
       </c>
@@ -2274,15 +2273,15 @@
         <v>43440</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="J31" s="28"/>
     </row>
@@ -2297,10 +2296,10 @@
         <v>43445</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
@@ -2314,7 +2313,7 @@
         <v>6</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2328,7 +2327,7 @@
   <dimension ref="A1:V82"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2348,9 +2347,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
@@ -2361,10 +2358,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -2395,17 +2392,17 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
       <c r="B2" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="10">
         <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>0</v>
@@ -2416,7 +2413,7 @@
       </c>
       <c r="J2" s="9">
         <f>I2/$I$7</f>
-        <v>0.26470588235294118</v>
+        <v>0.25714285714285712</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>0</v>
@@ -2438,17 +2435,17 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
       <c r="B3" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="10">
         <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>7</v>
@@ -2459,7 +2456,7 @@
       </c>
       <c r="J3" s="12">
         <f>I3/$I$7</f>
-        <v>0.19117647058823528</v>
+        <v>0.18571428571428572</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>7</v>
@@ -2481,17 +2478,17 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2.2000000000000002</v>
-      </c>
       <c r="B4" s="24" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="6">
         <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>4</v>
@@ -2502,7 +2499,7 @@
       </c>
       <c r="J4" s="16">
         <f>I4/$I$7</f>
-        <v>0.14705882352941177</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>4</v>
@@ -2524,17 +2521,17 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
       <c r="B5" s="25" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="10">
         <v>10</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>8</v>
@@ -2545,7 +2542,7 @@
       </c>
       <c r="J5" s="22">
         <f>I5/$I$7</f>
-        <v>0.10294117647058823</v>
+        <v>0.1</v>
       </c>
       <c r="P5" s="20" t="s">
         <v>8</v>
@@ -2567,11 +2564,8 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>3.2</v>
-      </c>
       <c r="B6" s="25" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>7</v>
@@ -2579,16 +2573,19 @@
       <c r="D6" s="6">
         <v>3</v>
       </c>
+      <c r="F6" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="H6" s="17" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="13">
         <f>SUMIF($C$2:$C$73,H6,$D$2:$D$73)</f>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="J6" s="18">
         <f>I6/$I$7</f>
-        <v>0.29411764705882354</v>
+        <v>0.31428571428571428</v>
       </c>
       <c r="P6" s="17" t="s">
         <v>5</v>
@@ -2605,11 +2602,8 @@
       <c r="V6" s="4"/>
     </row>
     <row r="7" spans="1:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>4</v>
-      </c>
       <c r="B7" s="24" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>0</v>
@@ -2617,9 +2611,12 @@
       <c r="D7" s="10">
         <v>10</v>
       </c>
+      <c r="F7" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="Q7" s="19">
         <f>SUM(Q2:Q6)</f>
@@ -2628,11 +2625,8 @@
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>4.2</v>
-      </c>
       <c r="B8" s="25" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>7</v>
@@ -2640,41 +2634,41 @@
       <c r="D8" s="6">
         <v>3</v>
       </c>
+      <c r="F8" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>4.3</v>
-      </c>
       <c r="B9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6">
         <v>5</v>
       </c>
-      <c r="D9" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="26">
-        <v>6</v>
+      <c r="F10" s="5" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>5</v>
-      </c>
       <c r="B11" s="25" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>0</v>
@@ -2682,55 +2676,55 @@
       <c r="D11" s="10">
         <v>10</v>
       </c>
+      <c r="F11" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>5.0999999999999996</v>
-      </c>
       <c r="B12" s="25" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="6">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>5.2</v>
-      </c>
       <c r="B13" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="13">
-        <v>20</v>
+        <v>161</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>5.3</v>
-      </c>
       <c r="B14" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="26">
-        <v>6</v>
+      <c r="D14" s="6">
+        <v>3</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>8</v>
-      </c>
       <c r="B15" s="25" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>0</v>
@@ -2738,163 +2732,193 @@
       <c r="D15" s="10">
         <v>10</v>
       </c>
+      <c r="F15" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>8.1</v>
-      </c>
       <c r="B16" s="25" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="6">
+        <v>3</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6">
+        <v>3</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="13">
+        <v>20</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="26">
         <v>6</v>
       </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="F20" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D21" s="13">
         <v>20</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="26" t="s">
+      <c r="F21" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C22" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D22" s="26">
         <v>6</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="10">
+      <c r="F22" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="13">
+        <v>20</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="26">
+        <v>6</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="13">
+        <v>20</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="26">
+        <v>6</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="13">
         <v>10</v>
       </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="6">
-        <v>3</v>
-      </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="10">
-        <v>10</v>
-      </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="6">
-        <v>3</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="10">
-        <v>10</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="13">
-        <v>10</v>
-      </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="26">
-        <v>6</v>
-      </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="25" t="s">
+      <c r="F27" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="25" t="s">
         <v>16</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="13">
-        <v>10</v>
-      </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="6">
-        <v>3</v>
-      </c>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
-        <v>17</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>7</v>
@@ -2902,11 +2926,14 @@
       <c r="D28" s="26">
         <v>6</v>
       </c>
+      <c r="F28" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>5</v>
@@ -2914,21 +2941,27 @@
       <c r="D29" s="13">
         <v>20</v>
       </c>
+      <c r="F29" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="26">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
         <v>6</v>
       </c>
@@ -2938,14 +2971,14 @@
       <c r="D31" s="15">
         <v>50</v>
       </c>
+      <c r="F31" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>0</v>
-      </c>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="24" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>8</v>
@@ -2953,9 +2986,11 @@
       <c r="D32" s="21">
         <v>35</v>
       </c>
+      <c r="F32" s="5" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="24"/>
       <c r="F36" s="5"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -2966,7 +3001,6 @@
       <c r="P36" s="3"/>
     </row>
     <row r="37" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="24"/>
       <c r="F37" s="5"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -2977,7 +3011,6 @@
       <c r="P37" s="3"/>
     </row>
     <row r="38" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="24"/>
       <c r="F38" s="5"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -2988,7 +3021,6 @@
       <c r="P38" s="3"/>
     </row>
     <row r="39" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="24"/>
       <c r="F39" s="5"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -2999,7 +3031,6 @@
       <c r="P39" s="3"/>
     </row>
     <row r="40" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="24"/>
       <c r="F40" s="5"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -3010,7 +3041,6 @@
       <c r="P40" s="3"/>
     </row>
     <row r="41" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="24"/>
       <c r="F41" s="5"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -3021,7 +3051,6 @@
       <c r="P41" s="3"/>
     </row>
     <row r="42" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="24"/>
       <c r="F42" s="5"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -3032,7 +3061,6 @@
       <c r="P42" s="3"/>
     </row>
     <row r="43" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="24"/>
       <c r="F43" s="5"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -3043,7 +3071,6 @@
       <c r="P43" s="3"/>
     </row>
     <row r="44" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="24"/>
       <c r="F44" s="5"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -3054,7 +3081,6 @@
       <c r="P44" s="3"/>
     </row>
     <row r="45" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="24"/>
       <c r="F45" s="5"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -3065,7 +3091,6 @@
       <c r="P45" s="3"/>
     </row>
     <row r="46" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="24"/>
       <c r="F46" s="5"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>

</xml_diff>

<commit_message>
enhance schedule and update lec02
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DA29F5-C19B-4574-BDEA-B37B2C883991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D520ED-9834-402C-8DCA-DD3AA50C7AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>Logistic Regression analysis</t>
   </si>
   <si>
-    <t>Project Stage IV: Multivariable Analysis &amp; Conclusions</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -245,11 +242,6 @@
   </si>
   <si>
     <t>collab</t>
-  </si>
-  <si>
-    <t>[Syllabus](../syllabus.html)
-[Help page](../help.html)
-PMA6 Ch 2</t>
   </si>
   <si>
     <t>week</t>
@@ -279,9 +271,6 @@
 There is a difference between human readable and computer readable data formats</t>
   </si>
   <si>
-    <t>Project Stage 1: Choosing your topic</t>
-  </si>
-  <si>
     <t>t08_mv_inf</t>
   </si>
   <si>
@@ -292,10 +281,6 @@
   </si>
   <si>
     <t>t11_exp_design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Write down several research questions
-</t>
   </si>
   <si>
     <t>Asking questions is easy. Asking _answerable_ questions is more difficult.</t>
@@ -306,10 +291,6 @@
   </si>
   <si>
     <t>[How to Write an Effective Research Question](https://library.csuchico.edu/library-curricula)</t>
-  </si>
-  <si>
-    <t>PMA6 Ch 3
-ASCN Ch 1</t>
   </si>
   <si>
     <t>Know several questions to ask yourself when preparing data for analysis
@@ -397,9 +378,6 @@
   </si>
   <si>
     <t xml:space="preserve">Create appropriate summary statistics and visualizations for combinations of two measures. </t>
-  </si>
-  <si>
-    <t>If all else fails, use "significant at p&gt;.05 level" and hope no one notices. Ref: https://xkcd.com/1478/</t>
   </si>
   <si>
     <t>Describing relationships between two variables</t>
@@ -576,19 +554,40 @@
     <t>[Poster prep Stage 2](project.html)</t>
   </si>
   <si>
-    <t>Project Stage 3: Exploratory Data Analysis</t>
-  </si>
-  <si>
     <t>[Poster prep Stage 3](project.html)</t>
   </si>
   <si>
-    <t>Project Stage 2: Introduce your research question and variables of interest</t>
-  </si>
-  <si>
-    <t>Project Stage 4: Bivariate Inference</t>
-  </si>
-  <si>
     <t>Other types of models</t>
+  </si>
+  <si>
+    <t>[Syllabus](../syllabus.html)  
+[Help page](../help.html)   
+PMA6 Ch 2</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 3  
+ASCN Ch 1</t>
+  </si>
+  <si>
+    <t>[If all else fails, use "significant at p&gt;.05 level" and hope no one notices.](https://xkcd.com/1478/)</t>
+  </si>
+  <si>
+    <t>**Project Stage 1:** Choosing your topic</t>
+  </si>
+  <si>
+    <t>**Project Stage IV:** Multivariable Analysis &amp; Conclusions</t>
+  </si>
+  <si>
+    <t>**Project Stage 4: **Bivariate Inference</t>
+  </si>
+  <si>
+    <t>**Project Stage 2:** Introduce your research question and variables of interest</t>
+  </si>
+  <si>
+    <t>**Project Stage 3:** Exploratory Data Analysis</t>
+  </si>
+  <si>
+    <t>Write down several research questions</t>
   </si>
 </sst>
 </file>
@@ -1485,8 +1484,8 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1506,40 +1505,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="37" t="s">
         <v>68</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1553,31 +1552,31 @@
         <v>43333</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>67</v>
+        <v>163</v>
       </c>
       <c r="J2" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K2" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" s="42" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
@@ -1588,29 +1587,29 @@
         <v>43333</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J3" s="45"/>
       <c r="K3" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -1622,10 +1621,10 @@
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="53" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
@@ -1645,29 +1644,29 @@
         <v>43340</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>81</v>
+        <v>171</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I5" s="56" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="41" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1678,29 +1677,29 @@
         <v>43342</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H6" s="41" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I6" s="41" t="s">
-        <v>85</v>
+        <v>164</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="41" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1715,7 +1714,7 @@
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="50" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="41"/>
@@ -1734,10 +1733,10 @@
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="50" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G8" s="41"/>
       <c r="H8" s="41"/>
@@ -1757,27 +1756,27 @@
         <v>43354</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G9" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="41" t="s">
         <v>93</v>
-      </c>
-      <c r="H9" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="I9" s="41" t="s">
-        <v>98</v>
       </c>
       <c r="J9" s="44"/>
       <c r="K9" s="44"/>
       <c r="L9" s="42" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1798,7 +1797,7 @@
       <c r="J10" s="48"/>
       <c r="K10" s="49"/>
       <c r="L10" s="53" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1812,27 +1811,27 @@
         <v>43361</v>
       </c>
       <c r="D11" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>111</v>
-      </c>
       <c r="G11" s="41" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I11" s="41" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="J11" s="44"/>
       <c r="K11" s="44"/>
       <c r="L11" s="42" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1846,17 +1845,17 @@
         <v>43368</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="41" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="J12" s="28"/>
       <c r="L12" s="29"/>
@@ -1870,7 +1869,7 @@
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
@@ -1879,7 +1878,7 @@
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="38" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
@@ -1893,24 +1892,24 @@
         <v>43375</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="41" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="41" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="L14" s="42"/>
     </row>
@@ -1922,28 +1921,28 @@
         <v>43377</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="I15" s="41" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="K15" s="41" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="L15" s="40"/>
     </row>
@@ -1959,10 +1958,10 @@
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="41" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="28"/>
@@ -1977,29 +1976,29 @@
         <v>43384</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H17" s="55" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="41" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="L17" s="50" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -2015,7 +2014,7 @@
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2028,7 +2027,7 @@
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
@@ -2048,12 +2047,12 @@
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
       <c r="I20" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J20" s="28"/>
     </row>
@@ -2066,7 +2065,7 @@
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
@@ -2075,7 +2074,7 @@
       <c r="J21" s="38"/>
       <c r="K21" s="39"/>
       <c r="L21" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2089,17 +2088,17 @@
         <v>43403</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2111,7 +2110,7 @@
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F23" s="28"/>
       <c r="L23" s="29"/>
@@ -2128,17 +2127,17 @@
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
       <c r="I24" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J24" s="28"/>
       <c r="L24" s="29" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2150,7 +2149,7 @@
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
@@ -2175,11 +2174,11 @@
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J26" s="28"/>
       <c r="L26" s="29" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2193,11 +2192,11 @@
         <v>21</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H27" s="28"/>
       <c r="I27" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J27" s="28"/>
       <c r="L27" s="29"/>
@@ -2211,7 +2210,7 @@
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
@@ -2220,7 +2219,7 @@
       <c r="J28" s="38"/>
       <c r="K28" s="39"/>
       <c r="L28" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2234,15 +2233,15 @@
         <v>43431</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J29" s="28"/>
     </row>
@@ -2257,12 +2256,12 @@
         <v>43438</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
       <c r="L30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2273,15 +2272,15 @@
         <v>43440</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J31" s="28"/>
     </row>
@@ -2299,7 +2298,7 @@
         <v>9</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
@@ -2313,7 +2312,7 @@
         <v>6</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2401,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>0</v>
@@ -2445,7 +2444,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>7</v>
@@ -2479,7 +2478,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -2488,7 +2487,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>4</v>
@@ -2522,7 +2521,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>0</v>
@@ -2531,7 +2530,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>8</v>
@@ -2565,7 +2564,7 @@
     </row>
     <row r="6" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>7</v>
@@ -2574,7 +2573,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>5</v>
@@ -2612,7 +2611,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
@@ -2626,7 +2625,7 @@
     </row>
     <row r="8" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>7</v>
@@ -2635,7 +2634,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2649,12 +2648,12 @@
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>7</v>
@@ -2663,12 +2662,12 @@
         <v>5</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>0</v>
@@ -2677,12 +2676,12 @@
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
@@ -2691,12 +2690,12 @@
         <v>3</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>0</v>
@@ -2705,12 +2704,12 @@
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>7</v>
@@ -2719,12 +2718,12 @@
         <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>0</v>
@@ -2733,12 +2732,12 @@
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>7</v>
@@ -2747,13 +2746,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>0</v>
@@ -2762,13 +2761,13 @@
         <v>10</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>7</v>
@@ -2777,13 +2776,13 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>5</v>
@@ -2792,13 +2791,13 @@
         <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>7</v>
@@ -2807,13 +2806,13 @@
         <v>6</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>5</v>
@@ -2822,13 +2821,13 @@
         <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>7</v>
@@ -2837,13 +2836,13 @@
         <v>6</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>5</v>
@@ -2852,13 +2851,13 @@
         <v>20</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>7</v>
@@ -2867,13 +2866,13 @@
         <v>6</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>5</v>
@@ -2882,13 +2881,13 @@
         <v>20</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>7</v>
@@ -2897,7 +2896,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -2912,7 +2911,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2927,7 +2926,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -2942,7 +2941,7 @@
         <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -2957,7 +2956,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -2972,13 +2971,13 @@
         <v>50</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>8</v>
@@ -2987,7 +2986,7 @@
         <v>35</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add R info to DM slides
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D520ED-9834-402C-8DCA-DD3AA50C7AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04256E85-7DA8-4106-A913-84702D848D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -565,29 +565,30 @@
 PMA6 Ch 2</t>
   </si>
   <si>
+    <t>[If all else fails, use "significant at p&gt;.05 level" and hope no one notices.](https://xkcd.com/1478/)</t>
+  </si>
+  <si>
+    <t>**Project Stage 1:** Choosing your topic</t>
+  </si>
+  <si>
+    <t>**Project Stage IV:** Multivariable Analysis &amp; Conclusions</t>
+  </si>
+  <si>
+    <t>**Project Stage 4: **Bivariate Inference</t>
+  </si>
+  <si>
+    <t>**Project Stage 2:** Introduce your research question and variables of interest</t>
+  </si>
+  <si>
+    <t>**Project Stage 3:** Exploratory Data Analysis</t>
+  </si>
+  <si>
+    <t>Write down several research questions</t>
+  </si>
+  <si>
     <t>PMA6 Ch 3  
-ASCN Ch 1</t>
-  </si>
-  <si>
-    <t>[If all else fails, use "significant at p&gt;.05 level" and hope no one notices.](https://xkcd.com/1478/)</t>
-  </si>
-  <si>
-    <t>**Project Stage 1:** Choosing your topic</t>
-  </si>
-  <si>
-    <t>**Project Stage IV:** Multivariable Analysis &amp; Conclusions</t>
-  </si>
-  <si>
-    <t>**Project Stage 4: **Bivariate Inference</t>
-  </si>
-  <si>
-    <t>**Project Stage 2:** Introduce your research question and variables of interest</t>
-  </si>
-  <si>
-    <t>**Project Stage 3:** Exploratory Data Analysis</t>
-  </si>
-  <si>
-    <t>Write down several research questions</t>
+ASCN Ch 1  
+[Project Structure by Danielle Navarro](https://slides.djnavarro.net/)</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1486,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1621,7 +1622,7 @@
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F4" s="54" t="s">
         <v>67</v>
@@ -1653,7 +1654,7 @@
         <v>78</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H5" s="41" t="s">
         <v>95</v>
@@ -1692,7 +1693,7 @@
         <v>94</v>
       </c>
       <c r="I6" s="41" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="41" t="s">
@@ -1788,7 +1789,7 @@
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F10" s="53"/>
       <c r="G10" s="53"/>
@@ -1869,7 +1870,7 @@
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
@@ -1927,7 +1928,7 @@
         <v>127</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G15" s="41" t="s">
         <v>143</v>
@@ -2065,7 +2066,7 @@
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
@@ -2210,7 +2211,7 @@
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>

</xml_diff>

<commit_message>
add notes for tomorrow
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04256E85-7DA8-4106-A913-84702D848D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AD7935-7257-404F-8713-DB9BC990B31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -458,13 +458,7 @@
     <t>lec06-data_viz_bestpractice</t>
   </si>
   <si>
-    <t>Best practices in Data Visualization</t>
-  </si>
-  <si>
     <t>Just because you can add it to a graph, doesn't mean you should.</t>
-  </si>
-  <si>
-    <t>PMA6 Ch 4.6</t>
   </si>
   <si>
     <t>[Choosing appropriate analysis](https://hackmd.io/@norcalbiostat/08-choosing-analysis)</t>
@@ -589,6 +583,13 @@
     <t>PMA6 Ch 3  
 ASCN Ch 1  
 [Project Structure by Danielle Navarro](https://slides.djnavarro.net/)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best practices in Data Visualization </t>
+  </si>
+  <si>
+    <t>PMA6 Ch 4.6  
+[Slides](https://math615.netlify.app/slides/lec06-data_viz_bestpractice.html)</t>
   </si>
 </sst>
 </file>
@@ -1485,8 +1486,8 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1568,7 +1569,7 @@
         <v>64</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J2" s="45" t="s">
         <v>51</v>
@@ -1622,7 +1623,7 @@
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="53" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F4" s="54" t="s">
         <v>67</v>
@@ -1654,7 +1655,7 @@
         <v>78</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H5" s="41" t="s">
         <v>95</v>
@@ -1693,7 +1694,7 @@
         <v>94</v>
       </c>
       <c r="I6" s="41" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="41" t="s">
@@ -1789,7 +1790,7 @@
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="53" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F10" s="53"/>
       <c r="G10" s="53"/>
@@ -1798,7 +1799,7 @@
       <c r="J10" s="48"/>
       <c r="K10" s="49"/>
       <c r="L10" s="53" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1835,7 +1836,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -1845,18 +1846,19 @@
       <c r="C12" s="31">
         <v>43368</v>
       </c>
+      <c r="D12" s="41"/>
       <c r="E12" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12" s="41" t="s">
         <v>132</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>133</v>
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="41" t="s">
         <v>131</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="J12" s="28"/>
       <c r="L12" s="29"/>
@@ -1870,7 +1872,7 @@
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
@@ -1879,7 +1881,7 @@
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
@@ -1928,10 +1930,10 @@
         <v>127</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H15" s="41" t="s">
         <v>124</v>
@@ -1962,7 +1964,7 @@
         <v>128</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="28"/>
@@ -1983,23 +1985,23 @@
         <v>130</v>
       </c>
       <c r="F17" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="H17" s="55" t="s">
-        <v>137</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="41" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L17" s="50" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -2066,7 +2068,7 @@
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
@@ -2099,7 +2101,7 @@
         <v>26</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2138,7 +2140,7 @@
       </c>
       <c r="J24" s="28"/>
       <c r="L24" s="29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2179,7 +2181,7 @@
       </c>
       <c r="J26" s="28"/>
       <c r="L26" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2211,7 +2213,7 @@
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
@@ -2273,7 +2275,7 @@
         <v>43440</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28" t="s">
@@ -2402,7 +2404,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>0</v>
@@ -2445,7 +2447,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>7</v>
@@ -2488,7 +2490,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>4</v>
@@ -2531,7 +2533,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>8</v>
@@ -2574,7 +2576,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>5</v>
@@ -2612,7 +2614,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
@@ -2635,7 +2637,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2649,7 +2651,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -2663,12 +2665,12 @@
         <v>5</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>0</v>
@@ -2677,12 +2679,12 @@
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
@@ -2691,12 +2693,12 @@
         <v>3</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>0</v>
@@ -2705,7 +2707,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -2719,12 +2721,12 @@
         <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>0</v>
@@ -2733,7 +2735,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -2747,13 +2749,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>0</v>
@@ -2762,7 +2764,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -2777,13 +2779,13 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>5</v>
@@ -2792,13 +2794,13 @@
         <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>7</v>
@@ -2807,13 +2809,13 @@
         <v>6</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>5</v>
@@ -2822,13 +2824,13 @@
         <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>7</v>
@@ -2837,13 +2839,13 @@
         <v>6</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>5</v>
@@ -2852,13 +2854,13 @@
         <v>20</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>7</v>
@@ -2867,13 +2869,13 @@
         <v>6</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>5</v>
@@ -2882,13 +2884,13 @@
         <v>20</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>7</v>
@@ -2897,7 +2899,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -2912,7 +2914,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2927,7 +2929,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -2942,7 +2944,7 @@
         <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -2957,7 +2959,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -2972,7 +2974,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I31" s="3"/>
     </row>
@@ -2987,7 +2989,7 @@
         <v>35</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
work on biv inf lec
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB24174E-0856-40FE-88F6-A55C88103DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A975BC4-1927-4A8D-B7D3-D7678D9762FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -449,9 +449,6 @@
 </t>
   </si>
   <si>
-    <t>t08_bivariate_modeling</t>
-  </si>
-  <si>
     <t>Modeling Bivariate relationships</t>
   </si>
   <si>
@@ -590,6 +587,9 @@
   <si>
     <t>PMA6 Ch 4.6  
 [Slides](https://math615.netlify.app/slides/lec06-data_viz_bestpractice.html)</t>
+  </si>
+  <si>
+    <t>t08-bivariate_modeling</t>
   </si>
 </sst>
 </file>
@@ -1486,8 +1486,8 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1569,7 +1569,7 @@
         <v>64</v>
       </c>
       <c r="I2" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J2" s="45" t="s">
         <v>51</v>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F4" s="54" t="s">
         <v>67</v>
@@ -1655,7 +1655,7 @@
         <v>78</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H5" s="41" t="s">
         <v>95</v>
@@ -1694,7 +1694,7 @@
         <v>94</v>
       </c>
       <c r="I6" s="41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J6" s="44"/>
       <c r="K6" s="41" t="s">
@@ -1790,7 +1790,7 @@
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F10" s="53"/>
       <c r="G10" s="53"/>
@@ -1799,7 +1799,7 @@
       <c r="J10" s="48"/>
       <c r="K10" s="49"/>
       <c r="L10" s="53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1848,17 +1848,17 @@
       </c>
       <c r="D12" s="41"/>
       <c r="E12" s="41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J12" s="28"/>
       <c r="L12" s="29"/>
@@ -1872,7 +1872,7 @@
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
@@ -1881,7 +1881,7 @@
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
@@ -1930,10 +1930,10 @@
         <v>127</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H15" s="41" t="s">
         <v>124</v>
@@ -1964,7 +1964,7 @@
         <v>128</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="28"/>
@@ -1979,29 +1979,29 @@
         <v>43384</v>
       </c>
       <c r="D17" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="E17" s="41" t="s">
         <v>129</v>
       </c>
-      <c r="E17" s="41" t="s">
-        <v>130</v>
-      </c>
       <c r="F17" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="H17" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="H17" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L17" s="50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
@@ -2101,7 +2101,7 @@
         <v>26</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="J24" s="28"/>
       <c r="L24" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="J26" s="28"/>
       <c r="L26" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
@@ -2275,7 +2275,7 @@
         <v>43440</v>
       </c>
       <c r="E31" s="47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28" t="s">
@@ -2329,7 +2329,7 @@
   <dimension ref="A1:V82"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" activeCellId="5" sqref="D19 D21 D23 D25 D29 D27"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2404,7 +2404,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>0</v>
@@ -2447,7 +2447,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>7</v>
@@ -2490,7 +2490,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>4</v>
@@ -2533,7 +2533,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>8</v>
@@ -2576,7 +2576,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>5</v>
@@ -2614,7 +2614,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
@@ -2637,7 +2637,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2651,7 +2651,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -2662,15 +2662,15 @@
         <v>7</v>
       </c>
       <c r="D10" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>0</v>
@@ -2679,26 +2679,26 @@
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>0</v>
@@ -2707,7 +2707,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -2721,12 +2721,12 @@
         <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>0</v>
@@ -2735,7 +2735,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -2749,13 +2749,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>0</v>
@@ -2764,7 +2764,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -2779,13 +2779,13 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>5</v>
@@ -2794,13 +2794,13 @@
         <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>7</v>
@@ -2809,13 +2809,13 @@
         <v>6</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>5</v>
@@ -2824,13 +2824,13 @@
         <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>7</v>
@@ -2839,13 +2839,13 @@
         <v>6</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>5</v>
@@ -2854,13 +2854,13 @@
         <v>20</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>7</v>
@@ -2869,13 +2869,13 @@
         <v>6</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>5</v>
@@ -2884,13 +2884,13 @@
         <v>20</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>7</v>
@@ -2899,7 +2899,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -2914,7 +2914,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2929,7 +2929,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -2944,7 +2944,7 @@
         <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -2959,7 +2959,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -2974,7 +2974,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I31" s="3"/>
     </row>
@@ -2989,7 +2989,7 @@
         <v>35</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add quizzes to lec07
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A975BC4-1927-4A8D-B7D3-D7678D9762FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E05172-A91E-4E9D-8A88-7E1F408C8A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
     <sheet name="points" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="173">
   <si>
     <t>Assignment</t>
   </si>
@@ -465,9 +465,6 @@
   </si>
   <si>
     <t>lec08-bivariate_modeling</t>
-  </si>
-  <si>
-    <t>[HW06 Bivariate Modeling](hw/06_biv_modeling.html)</t>
   </si>
   <si>
     <t>06 Bivariate Inference</t>
@@ -590,6 +587,13 @@
   </si>
   <si>
     <t>t08-bivariate_modeling</t>
+  </si>
+  <si>
+    <t>[HW06 Bivariate Modeling](hw/hw06-biv_modeling.html)</t>
+  </si>
+  <si>
+    <t>[Quiz: Quantifying Uncertainty](https://forms.gle/PQGYizu45bCSoQAM9)
+[Quiz: Foundations for Inference](https://forms.gle/a4tEWsRf1nxkoz3P6)</t>
   </si>
 </sst>
 </file>
@@ -1006,9 +1010,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1056,6 +1057,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -1486,8 +1490,8 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1550,34 +1554,34 @@
       <c r="B2" s="27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C2" s="43">
+      <c r="C2" s="42">
         <v>43333</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="J2" s="45" t="s">
+      <c r="I2" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="41" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1585,55 +1589,55 @@
       <c r="B3" s="27">
         <v>1.2</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="42">
         <v>43333</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="45"/>
-      <c r="K3" s="41" t="s">
+      <c r="J3" s="44"/>
+      <c r="K3" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="41" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="51">
+      <c r="B4" s="50">
         <v>1.3</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="51">
         <v>43335</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="53" t="s">
-        <v>162</v>
-      </c>
-      <c r="F4" s="54" t="s">
+      <c r="D4" s="48"/>
+      <c r="E4" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="48"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -1642,32 +1646,32 @@
       <c r="B5" s="27">
         <v>2.1</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="42">
         <v>43340</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="H5" s="41" t="s">
+      <c r="G5" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="56" t="s">
+      <c r="I5" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="44"/>
-      <c r="K5" s="41" t="s">
+      <c r="J5" s="43"/>
+      <c r="K5" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="42" t="s">
+      <c r="L5" s="41" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1675,32 +1679,32 @@
       <c r="B6" s="27">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="42">
         <v>43342</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I6" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="J6" s="44"/>
-      <c r="K6" s="41" t="s">
+      <c r="I6" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="43"/>
+      <c r="K6" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="L6" s="42" t="s">
+      <c r="L6" s="41" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1711,41 +1715,41 @@
       <c r="B7" s="33">
         <v>3.1</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="42">
         <v>43347</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="50" t="s">
+      <c r="D7" s="44"/>
+      <c r="E7" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="46"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="33">
         <v>3.2</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="42">
         <v>43349</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="50" t="s">
+      <c r="D8" s="44"/>
+      <c r="E8" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="46"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="45"/>
     </row>
     <row r="9" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -1754,30 +1758,30 @@
       <c r="B9" s="27">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="42">
         <v>43354</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="42" t="s">
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="41" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1785,21 +1789,21 @@
       <c r="B10" s="27">
         <v>4.2</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="42">
         <v>43356</v>
       </c>
       <c r="D10" s="38"/>
-      <c r="E10" s="53" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="53" t="s">
-        <v>157</v>
+      <c r="E10" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="52" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1809,30 +1813,30 @@
       <c r="B11" s="27">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C11" s="43">
+      <c r="C11" s="42">
         <v>43361</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="F11" s="41" t="s">
+      <c r="F11" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="I11" s="41" t="s">
+      <c r="I11" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="42" t="s">
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="41" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1846,19 +1850,19 @@
       <c r="C12" s="31">
         <v>43368</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41" t="s">
+      <c r="D12" s="40"/>
+      <c r="E12" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="I12" s="40" t="s">
         <v>169</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>131</v>
-      </c>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="I12" s="41" t="s">
-        <v>170</v>
       </c>
       <c r="J12" s="28"/>
       <c r="L12" s="29"/>
@@ -1872,7 +1876,7 @@
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
@@ -1881,7 +1885,7 @@
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
@@ -1894,27 +1898,27 @@
       <c r="C14" s="31">
         <v>43375</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="40" t="s">
         <v>119</v>
       </c>
       <c r="H14" s="28"/>
-      <c r="I14" s="41" t="s">
+      <c r="I14" s="40" t="s">
         <v>126</v>
       </c>
       <c r="J14" s="28"/>
-      <c r="K14" s="41" t="s">
+      <c r="K14" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="L14" s="42"/>
+      <c r="L14" s="41"/>
     </row>
     <row r="15" spans="1:12" ht="220.5" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
@@ -1923,31 +1927,33 @@
       <c r="C15" s="31">
         <v>43377</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="E15" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="F15" s="41" t="s">
-        <v>161</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="H15" s="41" t="s">
+      <c r="F15" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="J15" s="41" t="s">
+      <c r="J15" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="K15" s="41" t="s">
+      <c r="K15" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="L15" s="40"/>
+      <c r="L15" s="56" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
@@ -1960,13 +1966,13 @@
         <v>43382</v>
       </c>
       <c r="D16" s="28"/>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="G16" s="41"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="28"/>
       <c r="J16" s="28"/>
       <c r="L16" s="29"/>
@@ -1978,30 +1984,30 @@
       <c r="C17" s="31">
         <v>43384</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J17" s="28"/>
+      <c r="K17" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="L17" s="40" t="s">
         <v>171</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="F17" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>138</v>
-      </c>
-      <c r="H17" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="L17" s="50" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -2068,7 +2074,7 @@
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
@@ -2101,7 +2107,7 @@
         <v>26</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2140,7 +2146,7 @@
       </c>
       <c r="J24" s="28"/>
       <c r="L24" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2181,7 +2187,7 @@
       </c>
       <c r="J26" s="28"/>
       <c r="L26" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2213,7 +2219,7 @@
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
@@ -2274,8 +2280,8 @@
       <c r="C31" s="31">
         <v>43440</v>
       </c>
-      <c r="E31" s="47" t="s">
-        <v>159</v>
+      <c r="E31" s="46" t="s">
+        <v>158</v>
       </c>
       <c r="F31" s="28"/>
       <c r="G31" s="28" t="s">
@@ -2404,7 +2410,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>0</v>
@@ -2447,7 +2453,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>7</v>
@@ -2490,7 +2496,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>4</v>
@@ -2533,7 +2539,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>8</v>
@@ -2576,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>5</v>
@@ -2614,7 +2620,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
@@ -2637,7 +2643,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2651,7 +2657,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -2665,12 +2671,12 @@
         <v>3</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>0</v>
@@ -2679,12 +2685,12 @@
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
@@ -2693,12 +2699,12 @@
         <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>0</v>
@@ -2707,7 +2713,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -2721,12 +2727,12 @@
         <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>0</v>
@@ -2735,7 +2741,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -2749,13 +2755,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>0</v>
@@ -2764,7 +2770,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -2779,13 +2785,13 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>5</v>
@@ -2794,13 +2800,13 @@
         <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>7</v>
@@ -2809,13 +2815,13 @@
         <v>6</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>5</v>
@@ -2824,13 +2830,13 @@
         <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>7</v>
@@ -2839,13 +2845,13 @@
         <v>6</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>5</v>
@@ -2854,13 +2860,13 @@
         <v>20</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>7</v>
@@ -2869,13 +2875,13 @@
         <v>6</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>5</v>
@@ -2884,13 +2890,13 @@
         <v>20</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>7</v>
@@ -2899,7 +2905,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -2914,7 +2920,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2929,7 +2935,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -2944,7 +2950,7 @@
         <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -2959,7 +2965,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -2974,7 +2980,7 @@
         <v>50</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I31" s="3"/>
     </row>
@@ -2989,7 +2995,7 @@
         <v>35</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finish correlation add regression
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D450AB-9399-49EC-8BDB-2983F352F647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2471D7C-A95F-4B0C-9E4C-63C363033BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="182">
   <si>
     <t>Assignment</t>
   </si>
@@ -110,21 +110,10 @@
   </si>
   <si>
     <t>03 RR / DM</t>
-  </si>
-  <si>
-    <t>PMA5 Ch 6
-ASCN Ch 7</t>
   </si>
   <si>
     <t>PMA5 Ch12
 ASCN Ch 10</t>
-  </si>
-  <si>
-    <t>ASCN 9.2, 9.3</t>
-  </si>
-  <si>
-    <t>PMA5 Ch 7
-ASCN Ch 8, 9.5</t>
   </si>
   <si>
     <t>PMA5 Ch8
@@ -386,9 +375,6 @@
     <t>Labor Day. No Class</t>
   </si>
   <si>
-    <t>Correlation &amp; Regression</t>
-  </si>
-  <si>
     <t>Moderation</t>
   </si>
   <si>
@@ -472,13 +458,6 @@
   <si>
     <t>Choosing appropriate analysis, 
 T-tests for difference in means</t>
-  </si>
-  <si>
-    <t>Identify the most appropriate analysis for a given research topic. 
-Fully conduct the following statistical analyses: Two sample T-Test of means, ANOVA,  Chi-squared test of Association, Correlation, Simple linear Regression</t>
-  </si>
-  <si>
-    <t>PMA6 Ch 6</t>
   </si>
   <si>
     <t>Explain how to test a hypothsis using randomization
@@ -600,6 +579,54 @@
   </si>
   <si>
     <t>Quiz: Chi-Square &amp; Regression</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>t09-regression</t>
+  </si>
+  <si>
+    <t>Linear Modeling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everything is a linear model. </t>
+  </si>
+  <si>
+    <t>PMA6 Ch 7  
+[ASCN Ch 7](https://norcalbiostat.github.io/AppliedStatistics_notes/reg-intro.html)  
+[IMS Ch 24](https://openintro-ims.netlify.app/inf-model-slr.html)</t>
+  </si>
+  <si>
+    <t>Identify the most appropriate analysis for a given research topic. 
+Fully conduct the following statistical analyses: Two sample T-Test of means, ANOVA,  Chi-squared test of Association, Correlation,</t>
+  </si>
+  <si>
+    <t>Use the least squares method to calculate an equation for a best fit line that describes the relationship between a continuous explanatory and continuous response variable  
+Calculate and interpret estimates for the intercept and slope of regression models 
+Use the regression equation to predict new values for Y given values of X
+Calculate and interpret confidence and prediction intervals for the slope value
+Visually assess assumptions of regression models</t>
+  </si>
+  <si>
+    <t>[IMS - Chapter 22](https://openintro-ims.netlify.app/inference-many-means.html)</t>
+  </si>
+  <si>
+    <t>[ASCN Ch 5](https://norcalbiostat.github.io/AppliedStatistics_notes/bivariate-analysis.html)
+IMS - Chapter 20](https://openintro-ims.netlify.app/inference-two-means.html)</t>
+  </si>
+  <si>
+    <t>ASCN 9.1</t>
+  </si>
+  <si>
+    <t>ASCN 9.2</t>
+  </si>
+  <si>
+    <t>ASCN 9.4</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 8
+ASCN Ch 8</t>
   </si>
 </sst>
 </file>
@@ -1493,11 +1520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1535,7 @@
     <col min="5" max="6" width="19.25" style="3" customWidth="1"/>
     <col min="7" max="7" width="40" style="3" customWidth="1"/>
     <col min="8" max="8" width="21" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22" style="3" customWidth="1"/>
+    <col min="9" max="9" width="23.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="17.625" style="3" customWidth="1"/>
     <col min="11" max="11" width="25.125" style="28" customWidth="1"/>
     <col min="12" max="12" width="19.375" style="3" customWidth="1"/>
@@ -1517,40 +1544,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I1" s="34" t="s">
         <v>22</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K1" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="37" t="s">
         <v>65</v>
-      </c>
-      <c r="L1" s="37" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1564,31 +1591,31 @@
         <v>43333</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F2" s="43" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I2" s="40" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J2" s="44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K2" s="40" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L2" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
@@ -1599,29 +1626,29 @@
         <v>43333</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J3" s="44"/>
       <c r="K3" s="40" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L3" s="41" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -1633,10 +1660,10 @@
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="52" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -1656,29 +1683,29 @@
         <v>43340</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I5" s="55" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J5" s="43"/>
       <c r="K5" s="40" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L5" s="41" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1689,29 +1716,29 @@
         <v>43342</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J6" s="43"/>
       <c r="K6" s="40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L6" s="41" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1726,7 +1753,7 @@
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="49" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
@@ -1745,10 +1772,10 @@
       </c>
       <c r="D8" s="44"/>
       <c r="E8" s="49" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
@@ -1768,27 +1795,27 @@
         <v>43354</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I9" s="40" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J9" s="43"/>
       <c r="K9" s="43"/>
       <c r="L9" s="41" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1800,7 +1827,7 @@
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="52" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F10" s="52"/>
       <c r="G10" s="52"/>
@@ -1809,7 +1836,7 @@
       <c r="J10" s="47"/>
       <c r="K10" s="48"/>
       <c r="L10" s="52" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -1823,27 +1850,27 @@
         <v>43361</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F11" s="40" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I11" s="40" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J11" s="43"/>
       <c r="K11" s="43"/>
       <c r="L11" s="41" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
@@ -1858,17 +1885,17 @@
       </c>
       <c r="D12" s="40"/>
       <c r="E12" s="40" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G12" s="40"/>
       <c r="H12" s="40" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I12" s="40" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J12" s="28"/>
       <c r="L12" s="29"/>
@@ -1882,7 +1909,7 @@
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
@@ -1891,7 +1918,7 @@
       <c r="J13" s="38"/>
       <c r="K13" s="39"/>
       <c r="L13" s="38" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
@@ -1905,24 +1932,24 @@
         <v>43375</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F14" s="40" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="40" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="40" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="L14" s="41"/>
     </row>
@@ -1934,31 +1961,31 @@
         <v>43377</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J15" s="40" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K15" s="40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="L15" s="56" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
@@ -1973,17 +2000,17 @@
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="40" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G16" s="40"/>
       <c r="H16" s="28"/>
       <c r="J16" s="28"/>
       <c r="L16" s="29"/>
     </row>
-    <row r="17" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="141.75" x14ac:dyDescent="0.25">
       <c r="B17" s="27">
         <v>8.1999999999999993</v>
       </c>
@@ -1991,32 +2018,32 @@
         <v>43384</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F17" s="40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="H17" s="54" t="s">
-        <v>134</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="I17" s="40" t="s">
+        <v>177</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="40" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L17" s="40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>9</v>
       </c>
@@ -2028,11 +2055,14 @@
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
-      <c r="F18" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>173</v>
+      <c r="F18" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="L18" s="40" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -2044,15 +2074,15 @@
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="28" t="s">
-        <v>47</v>
+      <c r="F19" s="40" t="s">
+        <v>44</v>
       </c>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
     </row>
-    <row r="20" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>10</v>
       </c>
@@ -2064,276 +2094,305 @@
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
-      <c r="F20" s="28" t="s">
-        <v>110</v>
+      <c r="F20" s="40" t="s">
+        <v>169</v>
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
-      <c r="I20" s="28" t="s">
-        <v>24</v>
-      </c>
+      <c r="I20" s="28"/>
       <c r="J20" s="28"/>
-      <c r="L20" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L20" s="28"/>
+    </row>
+    <row r="21" spans="1:12" ht="189" x14ac:dyDescent="0.25">
       <c r="B21" s="27">
         <v>10.199999999999999</v>
       </c>
       <c r="C21" s="31">
+        <v>43396</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="J21" s="28"/>
+      <c r="L21" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="27">
+        <v>10.3</v>
+      </c>
+      <c r="C22" s="31">
         <v>43398</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="38" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="D22" s="38"/>
+      <c r="E22" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>11</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B23" s="27">
         <v>11.1</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C23" s="31">
         <v>43403</v>
       </c>
-      <c r="E22" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L22" s="29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="27">
+      <c r="E23" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="L23" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="27">
         <v>11.2</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C24" s="31">
         <v>43405</v>
-      </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" s="28"/>
-      <c r="L23" s="29"/>
-    </row>
-    <row r="24" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>12</v>
-      </c>
-      <c r="B24" s="27">
-        <v>12.1</v>
-      </c>
-      <c r="C24" s="31">
-        <v>43410</v>
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="J24" s="28"/>
-      <c r="L24" s="29" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I24" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="L24" s="29"/>
+    </row>
+    <row r="25" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>12</v>
+      </c>
       <c r="B25" s="27">
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="C25" s="31">
-        <v>43412</v>
+        <v>43410</v>
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
+      <c r="I25" s="28" t="s">
+        <v>181</v>
+      </c>
       <c r="J25" s="28"/>
-      <c r="L25" s="29"/>
-    </row>
-    <row r="26" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>13</v>
-      </c>
+      <c r="L25" s="29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="27">
-        <v>13.1</v>
+        <v>12.2</v>
       </c>
       <c r="C26" s="31">
-        <v>43417</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>43412</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="28"/>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="28" t="s">
-        <v>29</v>
+        <v>180</v>
       </c>
       <c r="J26" s="28"/>
-      <c r="L26" s="29" t="s">
-        <v>141</v>
-      </c>
+      <c r="L26" s="29"/>
     </row>
     <row r="27" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>13</v>
+      </c>
       <c r="B27" s="27">
-        <v>13.2</v>
+        <v>13.1</v>
       </c>
       <c r="C27" s="31">
-        <v>43419</v>
+        <v>43417</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>75</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J27" s="28"/>
-      <c r="L27" s="29"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L27" s="29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B28" s="27">
-        <v>13.3</v>
+        <v>13.2</v>
       </c>
       <c r="C28" s="31">
         <v>43419</v>
       </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>14</v>
-      </c>
+      <c r="E28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="28"/>
+      <c r="L28" s="29"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="27">
-        <v>14.1</v>
+        <v>13.3</v>
       </c>
       <c r="C29" s="31">
-        <v>43431</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J29" s="28"/>
+        <v>43419</v>
+      </c>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="38" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
+        <v>14</v>
+      </c>
+      <c r="B30" s="27">
+        <v>14.1</v>
+      </c>
+      <c r="C30" s="31">
+        <v>43431</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" s="28"/>
+    </row>
+    <row r="31" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>15</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B31" s="27">
         <v>15.1</v>
       </c>
-      <c r="C30" s="31">
+      <c r="C31" s="31">
         <v>43438</v>
       </c>
-      <c r="E30" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="L30" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="27">
+      <c r="E31" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="L31" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="27">
         <v>15.2</v>
       </c>
-      <c r="C31" s="31">
+      <c r="C32" s="31">
         <v>43440</v>
       </c>
-      <c r="E31" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="J31" s="28"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="E32" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" s="28"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>16</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B33" s="27">
         <v>16.100000000000001</v>
       </c>
-      <c r="C32" s="31">
+      <c r="C33" s="31">
         <v>43445</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L32" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="27">
+      <c r="L33" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="27">
         <v>16.2</v>
       </c>
-      <c r="C33" s="31">
+      <c r="C34" s="31">
         <v>43449</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L33" s="3" t="s">
-        <v>40</v>
+      <c r="L34" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2422,7 +2481,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>0</v>
@@ -2465,7 +2524,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>7</v>
@@ -2499,7 +2558,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -2508,7 +2567,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>4</v>
@@ -2551,7 +2610,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>8</v>
@@ -2585,7 +2644,7 @@
     </row>
     <row r="6" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>7</v>
@@ -2594,7 +2653,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>5</v>
@@ -2632,7 +2691,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
@@ -2646,7 +2705,7 @@
     </row>
     <row r="8" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>7</v>
@@ -2655,7 +2714,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2669,12 +2728,12 @@
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>7</v>
@@ -2683,12 +2742,12 @@
         <v>3</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="25" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>0</v>
@@ -2697,12 +2756,12 @@
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>7</v>
@@ -2711,12 +2770,12 @@
         <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>0</v>
@@ -2725,12 +2784,12 @@
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>7</v>
@@ -2739,12 +2798,12 @@
         <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>0</v>
@@ -2753,12 +2812,12 @@
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>7</v>
@@ -2767,13 +2826,13 @@
         <v>3</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="25" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>0</v>
@@ -2782,13 +2841,13 @@
         <v>10</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>7</v>
@@ -2797,13 +2856,13 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>5</v>
@@ -2812,13 +2871,13 @@
         <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="25" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>7</v>
@@ -2827,13 +2886,13 @@
         <v>6</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="25" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>5</v>
@@ -2842,13 +2901,13 @@
         <v>20</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="25" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>7</v>
@@ -2857,13 +2916,13 @@
         <v>6</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="25" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>5</v>
@@ -2872,13 +2931,13 @@
         <v>20</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>7</v>
@@ -2887,13 +2946,13 @@
         <v>6</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>5</v>
@@ -2902,13 +2961,13 @@
         <v>20</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="25" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C26" s="26" t="s">
         <v>7</v>
@@ -2917,7 +2976,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I26" s="3"/>
     </row>
@@ -2932,7 +2991,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -2947,7 +3006,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -2962,7 +3021,7 @@
         <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -2977,7 +3036,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -2992,13 +3051,13 @@
         <v>50</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>8</v>
@@ -3007,7 +3066,7 @@
         <v>35</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add slides to schedule
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2471D7C-A95F-4B0C-9E4C-63C363033BE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66D967D-2223-49E0-9BE1-7828EF9AF793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="183">
   <si>
     <t>Assignment</t>
   </si>
@@ -627,6 +627,9 @@
   <si>
     <t>PMA6 Ch 8
 ASCN Ch 8</t>
+  </si>
+  <si>
+    <t>[Bivariate inference slides continued](https://math615.netlify.app/slides/lec08-bivariate_modeling.html#/simple-linear-regression)</t>
   </si>
 </sst>
 </file>
@@ -1523,8 +1526,8 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2122,7 +2125,9 @@
       <c r="G21" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="H21" s="40"/>
+      <c r="H21" s="40" t="s">
+        <v>182</v>
+      </c>
       <c r="I21" s="40" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
add week topic page
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BFF33D-58F5-47FD-A5A3-BC2A4950ACC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667D329D-E0D4-44AF-9487-59540E2FBCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="189">
   <si>
     <t>Assignment</t>
   </si>
@@ -509,11 +509,6 @@
     <t xml:space="preserve">Everything is a linear model. </t>
   </si>
   <si>
-    <t>PMA6 Ch 7  
-[ASCN Ch 7](https://norcalbiostat.github.io/AppliedStatistics_notes/reg-intro.html)  
-[IMS Ch 24](https://openintro-ims.netlify.app/inf-model-slr.html)</t>
-  </si>
-  <si>
     <t>Identify the most appropriate analysis for a given research topic. 
 Fully conduct the following statistical analyses: Two sample T-Test of means, ANOVA,  Chi-squared test of Association, Correlation,</t>
   </si>
@@ -547,13 +542,6 @@
     <t>t10-mod_strat</t>
   </si>
   <si>
-    <t>ASCN Ch 8</t>
-  </si>
-  <si>
-    <t>PMA6 Ch 8
-ASCN Ch 9</t>
-  </si>
-  <si>
     <t>[HW06 Bivariate Modeling](hw06-biv_modeling.html)</t>
   </si>
   <si>
@@ -565,10 +553,6 @@
   </si>
   <si>
     <t>Generalized Linear Models</t>
-  </si>
-  <si>
-    <t>PMA6 Ch 12
-ASCN 11</t>
   </si>
   <si>
     <t>Calculate and interpret estimates for multiple slopes in multiple regression models 
@@ -599,10 +583,6 @@
     <t>t11-multiple_regression</t>
   </si>
   <si>
-    <t>PMA6 Ch 10.3
-ASCN 10.1, 10.2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Monday 6pm-8pm. </t>
   </si>
   <si>
@@ -616,9 +596,6 @@
   </si>
   <si>
     <t>**Project Stage 5:** Multivariable Analysis &amp; Conclusions</t>
-  </si>
-  <si>
-    <t>ASCN Ch 10</t>
   </si>
   <si>
     <t>[Poster Evaluation Rubric](https://forms.gle/SWBM96MjcEmMDHGo9)
@@ -641,6 +618,44 @@
   </si>
   <si>
     <t>Poster Code</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 7  
+[ASCN Ch 7](https://norcalbiostat.github.io/AppliedStatistics_notes/slr.html)  
+[IMS Ch 24](https://openintro-ims.netlify.app/inf-model-slr.html)</t>
+  </si>
+  <si>
+    <t>[ASCN Ch 8](https://norcalbiostat.github.io/AppliedStatistics_notes/mod-strat.html)</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 8
+[ASCN Ch 9](https://norcalbiostat.github.io/AppliedStatistics_notes/mlr.html)</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 10.3
+[ASCN 10.1, 10.2](https://norcalbiostat.github.io/AppliedStatistics_notes/model-building.html)</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 12
+[ASCN 11](https://norcalbiostat.github.io/AppliedStatistics_notes/glm.html)</t>
+  </si>
+  <si>
+    <t>Part science, part art</t>
+  </si>
+  <si>
+    <t>Fit a model with a binary outcome and interpret the results
+Fit a model with a log transformed outcome and interpret the results</t>
+  </si>
+  <si>
+    <t>Identify techniques for selecting variables to be included in a model
+Select between competing models using measures of model fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.9-11 (wls, paired, forecasting), </t>
+  </si>
+  <si>
+    <t>PMA6 8.11, 9
+ASCN Ch 10</t>
   </si>
 </sst>
 </file>
@@ -931,7 +946,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1104,8 +1119,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="83">
@@ -1536,8 +1554,8 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2040,20 +2058,20 @@
         <v>112</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H17" s="40" t="s">
         <v>110</v>
       </c>
       <c r="I17" s="40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="40" t="s">
         <v>108</v>
       </c>
       <c r="L17" s="40" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="63" x14ac:dyDescent="0.25">
@@ -2072,7 +2090,7 @@
         <v>33</v>
       </c>
       <c r="I18" s="40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L18" s="40" t="s">
         <v>141</v>
@@ -2095,7 +2113,7 @@
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
       <c r="L19" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2136,17 +2154,17 @@
         <v>145</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H21" s="40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>146</v>
+        <v>179</v>
       </c>
       <c r="J21" s="28"/>
       <c r="L21" s="40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2167,7 +2185,7 @@
       <c r="J22" s="52"/>
       <c r="K22" s="53"/>
       <c r="L22" s="52" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="110.25" x14ac:dyDescent="0.25">
@@ -2181,25 +2199,25 @@
         <v>43403</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F23" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G23" s="40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H23" s="49"/>
       <c r="I23" s="40" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="J23" s="49"/>
       <c r="K23" s="40"/>
       <c r="L23" s="55" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
@@ -2213,27 +2231,27 @@
         <v>43410</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E24" s="40" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F24" s="40" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="40" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="J24" s="28"/>
       <c r="L24" s="55" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B25" s="27">
         <v>12.2</v>
       </c>
@@ -2246,16 +2264,16 @@
       </c>
       <c r="F25" s="49"/>
       <c r="G25" s="40" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H25" s="40"/>
       <c r="I25" s="40" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="J25" s="28"/>
       <c r="L25" s="29"/>
     </row>
-    <row r="26" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>13</v>
       </c>
@@ -2266,22 +2284,24 @@
         <v>43417</v>
       </c>
       <c r="E26" s="49" t="s">
+        <v>158</v>
+      </c>
+      <c r="F26" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="F26" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="G26" s="28"/>
+      <c r="G26" s="40" t="s">
+        <v>185</v>
+      </c>
       <c r="H26" s="28"/>
       <c r="I26" s="40" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="J26" s="28"/>
       <c r="L26" s="55" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>14</v>
       </c>
@@ -2291,29 +2311,34 @@
       <c r="C27" s="31">
         <v>43431</v>
       </c>
-      <c r="E27" s="46" t="s">
+      <c r="D27" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="E27" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="H27" s="28"/>
+      <c r="F27" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="H27" s="40"/>
       <c r="I27" s="40" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="27">
-        <v>14.2</v>
+        <v>14.3</v>
       </c>
       <c r="C28" s="31">
         <v>43431</v>
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
@@ -2322,7 +2347,7 @@
       <c r="J28" s="38"/>
       <c r="K28" s="39"/>
       <c r="L28" s="38" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2332,17 +2357,17 @@
       <c r="C29" s="31">
         <v>43433</v>
       </c>
-      <c r="D29" s="38"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="58" t="s">
-        <v>181</v>
-      </c>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="38"/>
+        <v>175</v>
+      </c>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="29"/>
     </row>
     <row r="30" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
@@ -2354,13 +2379,18 @@
       <c r="C30" s="31">
         <v>43438</v>
       </c>
-      <c r="E30" s="46" t="s">
+      <c r="D30" s="38"/>
+      <c r="E30" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="39"/>
       <c r="L30" s="38" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2374,7 +2404,9 @@
         <v>128</v>
       </c>
       <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
+      <c r="G31" s="28" t="s">
+        <v>187</v>
+      </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
       <c r="J31" s="28"/>
@@ -2393,10 +2425,10 @@
         <v>9</v>
       </c>
       <c r="G32" s="28" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
@@ -2411,7 +2443,7 @@
       </c>
       <c r="G33" s="28"/>
       <c r="L33" s="44" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3078,7 +3110,7 @@
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="25" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>5</v>
@@ -3120,7 +3152,7 @@
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="24" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C33" s="21" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
finish wk2 figure out what to do with slides
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219804A2-03AC-4BAB-A793-3728C1BF7EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BABB36-32E3-4FC5-A2CD-15CBBDB082E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="208">
   <si>
     <t>Assignment</t>
   </si>
@@ -703,7 +703,16 @@
     <t>https://hackmd.io/@norcalbiostat/03_dm</t>
   </si>
   <si>
-    <t>[Quiz 03]()</t>
+    <t>projecct</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>02_rq</t>
   </si>
 </sst>
 </file>
@@ -713,7 +722,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -830,6 +839,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1029,7 +1046,7 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1150,9 +1167,6 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="82" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="83"/>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="84"/>
@@ -1175,6 +1189,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="86" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="86" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1609,9 +1629,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:G6"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1663,7 +1683,7 @@
       <c r="K1" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="46" t="s">
         <v>42</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -1680,31 +1700,31 @@
       <c r="C2" s="33">
         <v>43697</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="43" t="s">
         <v>112</v>
       </c>
       <c r="J2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="49" t="s">
         <v>199</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="43" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1715,32 +1735,32 @@
       <c r="C3" s="33">
         <v>43697</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="43" t="s">
         <v>188</v>
       </c>
       <c r="J3" s="35"/>
-      <c r="K3" s="50" t="s">
+      <c r="K3" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="43" t="s">
         <v>200</v>
       </c>
     </row>
@@ -1773,55 +1793,53 @@
       <c r="B5" s="25">
         <v>2.1</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="48">
         <v>43704</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="G5" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="34"/>
-      <c r="K5" s="50" t="s">
+      <c r="J5" s="43"/>
+      <c r="K5" s="51" t="s">
         <v>196</v>
       </c>
-      <c r="L5" s="34" t="s">
+      <c r="L5" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="M5" s="34" t="s">
-        <v>202</v>
-      </c>
+      <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="25">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="48">
         <v>43706</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="43" t="s">
         <v>50</v>
       </c>
       <c r="H6" s="34" t="s">
@@ -1831,14 +1849,14 @@
         <v>119</v>
       </c>
       <c r="J6" s="34"/>
-      <c r="K6" s="50" t="s">
+      <c r="K6" s="49" t="s">
         <v>203</v>
       </c>
       <c r="L6" s="34" t="s">
         <v>65</v>
       </c>
       <c r="M6" s="34" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -2562,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB861DFA-F44D-408D-9771-0C086E04E7DE}">
   <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="116" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="B1" zoomScale="116" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2646,7 +2664,10 @@
       </c>
       <c r="J2" s="9">
         <f>I2/$I$7</f>
-        <v>0.27586206896551724</v>
+        <v>0.2807017543859649</v>
+      </c>
+      <c r="K2" s="4">
+        <v>30</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>0</v>
@@ -2686,7 +2707,10 @@
       </c>
       <c r="J3" s="12">
         <f>I3/$I$7</f>
-        <v>0.10344827586206896</v>
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="K3" s="4">
+        <v>10</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>7</v>
@@ -2722,11 +2746,14 @@
       </c>
       <c r="I4" s="15">
         <f>SUMIF($C$2:$C$66,H4,$D$2:$D$66)</f>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J4" s="16">
         <f>I4/$I$7</f>
-        <v>0.17241379310344829</v>
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="K4" s="4">
+        <v>10</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>4</v>
@@ -2762,11 +2789,14 @@
       </c>
       <c r="I5" s="21">
         <f>SUMIF($C$2:$C$66,H5,$D$2:$D$66)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J5" s="22">
         <f>I5/$I$7</f>
-        <v>0.17241379310344829</v>
+        <v>0.19298245614035087</v>
+      </c>
+      <c r="K5" s="4">
+        <v>20</v>
       </c>
       <c r="P5" s="20" t="s">
         <v>8</v>
@@ -2802,11 +2832,14 @@
       </c>
       <c r="I6" s="13">
         <f>SUMIF($C$2:$C$66,H6,$D$2:$D$66)</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="J6" s="18">
         <f>I6/$I$7</f>
-        <v>0.27586206896551724</v>
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="K6" s="4">
+        <v>30</v>
       </c>
       <c r="P6" s="17" t="s">
         <v>5</v>
@@ -2834,7 +2867,7 @@
       </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="Q7" s="19">
         <f>SUM(Q2:Q6)</f>
@@ -2890,7 +2923,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="13">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="40"/>
@@ -2916,7 +2949,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="13">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="40"/>
@@ -2942,7 +2975,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="13">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I16" s="3"/>
     </row>
@@ -2966,7 +2999,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="13">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="I18" s="3"/>
     </row>
@@ -3014,7 +3047,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="13">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="I22" s="3"/>
     </row>
@@ -3038,7 +3071,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="15">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I24" s="3"/>
     </row>
@@ -3050,7 +3083,7 @@
         <v>8</v>
       </c>
       <c r="D25" s="21">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
@@ -3413,109 +3446,135 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F574C0-FBB9-4BEB-B1DB-7DECF0319825}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="24.1875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="25.9375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" customWidth="1"/>
-    <col min="5" max="5" width="12.9375" style="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="45"/>
+    <col min="4" max="4" width="8.25" style="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="9" style="44"/>
+    <col min="7" max="7" width="12.9375" style="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="41" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A2" s="43" t="s">
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A2" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A4" s="48" t="s">
+      <c r="C2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A4" s="47" t="s">
         <v>192</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>191</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="47" t="s">
         <v>190</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="47" t="s">
         <v>189</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="F4" s="47" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4" s="47" t="s">
         <v>193</v>
       </c>
-      <c r="F4" s="48" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A5" s="42" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A5" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="41" t="s">
         <v>175</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="46" t="s">
+      <c r="D5" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="E5" s="41"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45" t="s">
         <v>185</v>
       </c>
-      <c r="F5" s="46"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A6" s="42" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A6" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="41" t="s">
         <v>186</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>185</v>
       </c>
       <c r="F6" s="45" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A7" s="42" t="s">
+      <c r="G6" s="45" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A7" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="41" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A8" s="42" t="s">
+      <c r="D7" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A8" s="41" t="s">
         <v>57</v>
       </c>
       <c r="B8" t="s">
@@ -3525,7 +3584,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -3536,7 +3595,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -3547,32 +3606,32 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
split lec03 notes into two sets of slides
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BABB36-32E3-4FC5-A2CD-15CBBDB082E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2356B9-08D2-43B9-BC6E-FC342F1D5572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="208">
   <si>
     <t>Assignment</t>
   </si>
@@ -424,11 +424,6 @@
     <t>Write down several research questions</t>
   </si>
   <si>
-    <t>PMA6 Ch 3  
-ASCN Ch 1  
-[Project Structure by Danielle Navarro](https://slides.djnavarro.net/)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Best practices in Data Visualization </t>
   </si>
   <si>
@@ -700,9 +695,6 @@
     <t>[Quiz 02]()</t>
   </si>
   <si>
-    <t>https://hackmd.io/@norcalbiostat/03_dm</t>
-  </si>
-  <si>
     <t>projecct</t>
   </si>
   <si>
@@ -713,6 +705,15 @@
   </si>
   <si>
     <t>02_rq</t>
+  </si>
+  <si>
+    <t>PMA6 Ch 3  
+ASCN Ch 1, Appendix 
+[Project Structure by Danielle Navarro](https://slides.djnavarro.net/)</t>
+  </si>
+  <si>
+    <t>lec03a-workflow   
+lec03b-data_prep</t>
   </si>
 </sst>
 </file>
@@ -722,7 +723,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -847,6 +848,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1046,7 +1054,7 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1195,6 +1203,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="86" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1629,9 +1640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1681,13 +1692,13 @@
         <v>22</v>
       </c>
       <c r="K1" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L1" s="46" t="s">
         <v>42</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="47.25" x14ac:dyDescent="0.5">
@@ -1722,7 +1733,7 @@
         <v>29</v>
       </c>
       <c r="K2" s="49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L2" s="43" t="s">
         <v>43</v>
@@ -1751,17 +1762,17 @@
         <v>63</v>
       </c>
       <c r="I3" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J3" s="35"/>
       <c r="K3" s="51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L3" s="43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M3" s="43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
@@ -1800,7 +1811,7 @@
         <v>56</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>48</v>
@@ -1809,14 +1820,14 @@
         <v>118</v>
       </c>
       <c r="H5" s="43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I5" s="50" t="s">
         <v>49</v>
       </c>
       <c r="J5" s="43"/>
       <c r="K5" s="51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L5" s="43" t="s">
         <v>64</v>
@@ -1842,21 +1853,19 @@
       <c r="G6" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="34" t="s">
-        <v>61</v>
+      <c r="H6" s="43" t="s">
+        <v>207</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="J6" s="34"/>
-      <c r="K6" s="49" t="s">
-        <v>203</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="J6" s="52"/>
+      <c r="K6" s="49"/>
       <c r="L6" s="34" t="s">
         <v>65</v>
       </c>
       <c r="M6" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -2003,7 +2012,7 @@
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>92</v>
@@ -2013,7 +2022,7 @@
         <v>91</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
@@ -2104,7 +2113,7 @@
         <v>84</v>
       </c>
       <c r="L15" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="47.25" x14ac:dyDescent="0.5">
@@ -2139,7 +2148,7 @@
         <v>43384</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>90</v>
@@ -2148,20 +2157,20 @@
         <v>97</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H17" s="34" t="s">
         <v>95</v>
       </c>
       <c r="I17" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J17" s="34"/>
       <c r="K17" s="34" t="s">
         <v>93</v>
       </c>
       <c r="L17" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="63" x14ac:dyDescent="0.5">
@@ -2182,12 +2191,12 @@
       <c r="G18" s="35"/>
       <c r="H18" s="35"/>
       <c r="I18" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J18" s="35"/>
       <c r="K18" s="34"/>
       <c r="L18" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="47.25" x14ac:dyDescent="0.5">
@@ -2208,7 +2217,7 @@
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.5">
@@ -2224,7 +2233,7 @@
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
       <c r="F20" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
@@ -2241,27 +2250,27 @@
         <v>43396</v>
       </c>
       <c r="D21" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="F21" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="F21" s="34" t="s">
-        <v>128</v>
-      </c>
       <c r="G21" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I21" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
       <c r="L21" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
@@ -2282,7 +2291,7 @@
       <c r="J22" s="36"/>
       <c r="K22" s="37"/>
       <c r="L22" s="37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="78.75" x14ac:dyDescent="0.5">
@@ -2296,25 +2305,25 @@
         <v>43403</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H23" s="35"/>
       <c r="I23" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J23" s="35"/>
       <c r="K23" s="34"/>
       <c r="L23" s="34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="94.5" x14ac:dyDescent="0.5">
@@ -2328,25 +2337,25 @@
         <v>43410</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G24" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H24" s="34"/>
       <c r="I24" s="34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J24" s="34"/>
       <c r="K24" s="34"/>
       <c r="L24" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="78.75" x14ac:dyDescent="0.5">
@@ -2362,11 +2371,11 @@
       </c>
       <c r="F25" s="35"/>
       <c r="G25" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H25" s="34"/>
       <c r="I25" s="34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J25" s="34"/>
       <c r="K25" s="34"/>
@@ -2384,22 +2393,22 @@
       </c>
       <c r="D26" s="35"/>
       <c r="E26" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H26" s="34"/>
       <c r="I26" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
       <c r="L26" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="63" x14ac:dyDescent="0.5">
@@ -2413,20 +2422,20 @@
         <v>43431</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E27" s="34" t="s">
         <v>76</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H27" s="34"/>
       <c r="I27" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J27" s="34"/>
       <c r="K27" s="34"/>
@@ -2441,7 +2450,7 @@
       </c>
       <c r="D28" s="36"/>
       <c r="E28" s="36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="36"/>
@@ -2450,7 +2459,7 @@
       <c r="J28" s="36"/>
       <c r="K28" s="37"/>
       <c r="L28" s="37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.5">
@@ -2462,7 +2471,7 @@
       </c>
       <c r="D29" s="35"/>
       <c r="E29" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F29" s="35"/>
       <c r="G29" s="35"/>
@@ -2493,7 +2502,7 @@
       <c r="J30" s="36"/>
       <c r="K30" s="37"/>
       <c r="L30" s="37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.5">
@@ -2509,7 +2518,7 @@
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
@@ -2533,14 +2542,14 @@
       </c>
       <c r="F32" s="35"/>
       <c r="G32" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H32" s="35"/>
       <c r="I32" s="35"/>
       <c r="J32" s="35"/>
       <c r="K32" s="34"/>
       <c r="L32" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.5">
@@ -2561,7 +2570,7 @@
       <c r="J33" s="35"/>
       <c r="K33" s="34"/>
       <c r="L33" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2569,10 +2578,9 @@
     <hyperlink ref="K5" r:id="rId1" xr:uid="{D7B4B181-09F4-4B83-A130-D70E0779356A}"/>
     <hyperlink ref="K3" r:id="rId2" xr:uid="{61C78E23-9C69-4897-BD30-D4F67D3BE011}"/>
     <hyperlink ref="K2" r:id="rId3" xr:uid="{552CE950-DBFD-451A-A563-A696EEACCA57}"/>
-    <hyperlink ref="K6" r:id="rId4" xr:uid="{13932CF6-1898-42A7-A0EE-531051BAF12A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2615,7 +2623,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -2904,7 +2912,7 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.5">
       <c r="B11" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>5</v>
@@ -3077,7 +3085,7 @@
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.5">
       <c r="B25" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C25" s="21" t="s">
         <v>8</v>
@@ -3464,48 +3472,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="41" t="s">
         <v>173</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>174</v>
       </c>
       <c r="D1" s="45"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>182</v>
-      </c>
       <c r="C2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4" s="47" t="s">
         <v>192</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>190</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>206</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>189</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="G4" s="47" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
@@ -3516,15 +3524,15 @@
         <v>39</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E5" s="41"/>
       <c r="F5" s="45"/>
       <c r="G5" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
@@ -3535,19 +3543,19 @@
         <v>63</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F6" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G6" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
@@ -3558,19 +3566,19 @@
         <v>62</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D7" s="45" t="s">
+        <v>203</v>
+      </c>
+      <c r="E7" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="E7" s="41" t="s">
-        <v>207</v>
-      </c>
       <c r="F7" s="45" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G7" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
@@ -3581,7 +3589,7 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
@@ -3589,10 +3597,10 @@
         <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.5">
@@ -3603,7 +3611,7 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
@@ -3618,27 +3626,27 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slight mod to project page
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\math615\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2356B9-08D2-43B9-BC6E-FC342F1D5572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161B88D2-0F2A-4A84-BBFE-E5E979DA3DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="208">
   <si>
     <t>Assignment</t>
   </si>
@@ -856,7 +856,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -924,6 +924,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1054,7 +1060,7 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1207,6 +1213,18 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="87">
@@ -1640,12 +1658,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.875" style="4"/>
     <col min="3" max="3" width="12" style="4" customWidth="1"/>
@@ -1660,7 +1678,7 @@
     <col min="13" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>40</v>
       </c>
@@ -1701,14 +1719,14 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="48">
         <v>43697</v>
       </c>
       <c r="D2" s="43" t="s">
@@ -1739,11 +1757,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="126" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" ht="126" x14ac:dyDescent="0.25">
       <c r="B3" s="25">
         <v>1.2</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="48">
         <v>43697</v>
       </c>
       <c r="D3" s="43" t="s">
@@ -1775,7 +1793,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="38">
         <v>1.3</v>
       </c>
@@ -1797,7 +1815,7 @@
       <c r="L4" s="37"/>
       <c r="M4" s="37"/>
     </row>
-    <row r="5" spans="1:13" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -1834,7 +1852,7 @@
       </c>
       <c r="M5" s="34"/>
     </row>
-    <row r="6" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="25">
         <v>2.2000000000000002</v>
       </c>
@@ -1868,7 +1886,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -1876,7 +1894,7 @@
         <v>3.1</v>
       </c>
       <c r="C7" s="33">
-        <v>43347</v>
+        <v>43711</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="35" t="s">
@@ -1890,12 +1908,12 @@
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
     </row>
-    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="29">
         <v>3.2</v>
       </c>
       <c r="C8" s="33">
-        <v>43349</v>
+        <v>43713</v>
       </c>
       <c r="D8" s="35"/>
       <c r="E8" s="35" t="s">
@@ -1911,7 +1929,7 @@
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
     </row>
-    <row r="9" spans="1:13" ht="63" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>4</v>
       </c>
@@ -1919,7 +1937,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C9" s="33">
-        <v>43354</v>
+        <v>43718</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>58</v>
@@ -1945,7 +1963,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B10" s="25">
         <v>4.2</v>
       </c>
@@ -1966,41 +1984,41 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="63" x14ac:dyDescent="0.5">
-      <c r="A11" s="4">
+    <row r="11" spans="1:13" s="56" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="53">
         <v>5</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="53">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="54">
         <v>43361</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34" t="s">
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>6</v>
       </c>
@@ -2028,7 +2046,7 @@
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
     </row>
-    <row r="13" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B13" s="25">
         <v>6.2</v>
       </c>
@@ -2049,7 +2067,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>7</v>
       </c>
@@ -2081,7 +2099,7 @@
       </c>
       <c r="L14" s="34"/>
     </row>
-    <row r="15" spans="1:13" ht="220.5" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" ht="220.5" x14ac:dyDescent="0.25">
       <c r="B15" s="25">
         <v>7.2</v>
       </c>
@@ -2116,7 +2134,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>8</v>
       </c>
@@ -2140,7 +2158,7 @@
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
     </row>
-    <row r="17" spans="1:12" ht="126" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:12" ht="141.75" x14ac:dyDescent="0.25">
       <c r="B17" s="25">
         <v>8.1999999999999993</v>
       </c>
@@ -2173,7 +2191,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="63" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>9</v>
       </c>
@@ -2199,7 +2217,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="25">
         <v>9.1999999999999993</v>
       </c>
@@ -2220,7 +2238,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>10</v>
       </c>
@@ -2242,7 +2260,7 @@
       <c r="K20" s="34"/>
       <c r="L20" s="34"/>
     </row>
-    <row r="21" spans="1:12" ht="189" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:12" ht="189" x14ac:dyDescent="0.25">
       <c r="B21" s="25">
         <v>10.199999999999999</v>
       </c>
@@ -2273,7 +2291,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B22" s="25">
         <v>10.3</v>
       </c>
@@ -2294,7 +2312,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>11</v>
       </c>
@@ -2326,7 +2344,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="94.5" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>12</v>
       </c>
@@ -2358,7 +2376,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B25" s="25">
         <v>12.2</v>
       </c>
@@ -2381,7 +2399,7 @@
       <c r="K25" s="34"/>
       <c r="L25" s="34"/>
     </row>
-    <row r="26" spans="1:12" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>13</v>
       </c>
@@ -2411,7 +2429,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="63" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>14</v>
       </c>
@@ -2441,7 +2459,7 @@
       <c r="K27" s="34"/>
       <c r="L27" s="34"/>
     </row>
-    <row r="28" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B28" s="25">
         <v>14.3</v>
       </c>
@@ -2462,7 +2480,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="25">
         <v>14.2</v>
       </c>
@@ -2481,7 +2499,7 @@
       <c r="K29" s="34"/>
       <c r="L29" s="34"/>
     </row>
-    <row r="30" spans="1:12" ht="63" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:12" ht="63" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>15</v>
       </c>
@@ -2505,7 +2523,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="25">
         <v>15.2</v>
       </c>
@@ -2526,7 +2544,7 @@
       <c r="K31" s="34"/>
       <c r="L31" s="34"/>
     </row>
-    <row r="32" spans="1:12" ht="94.5" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>16</v>
       </c>
@@ -2552,7 +2570,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="25">
         <v>16.2</v>
       </c>
@@ -2589,10 +2607,10 @@
   <dimension ref="A1:V75"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="116" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.875" style="4"/>
     <col min="2" max="2" width="36.875" style="24" bestFit="1" customWidth="1"/>
@@ -2608,7 +2626,7 @@
     <col min="12" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="23" t="s">
         <v>0</v>
@@ -2653,7 +2671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
@@ -2662,6 +2680,9 @@
       </c>
       <c r="D2" s="10">
         <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>0</v>
@@ -2672,7 +2693,7 @@
       </c>
       <c r="J2" s="9">
         <f>I2/$I$7</f>
-        <v>0.2807017543859649</v>
+        <v>0.2711864406779661</v>
       </c>
       <c r="K2" s="4">
         <v>30</v>
@@ -2696,7 +2717,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
         <v>12</v>
       </c>
@@ -2705,6 +2726,9 @@
       </c>
       <c r="D3" s="10">
         <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>7</v>
@@ -2715,7 +2739,7 @@
       </c>
       <c r="J3" s="12">
         <f>I3/$I$7</f>
-        <v>0.10526315789473684</v>
+        <v>0.10169491525423729</v>
       </c>
       <c r="K3" s="4">
         <v>10</v>
@@ -2739,7 +2763,7 @@
         <v>0.12698412698412698</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
         <v>21</v>
       </c>
@@ -2758,7 +2782,7 @@
       </c>
       <c r="J4" s="16">
         <f>I4/$I$7</f>
-        <v>0.10526315789473684</v>
+        <v>0.10169491525423729</v>
       </c>
       <c r="K4" s="4">
         <v>10</v>
@@ -2782,7 +2806,7 @@
         <v>0.31746031746031744</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
         <v>19</v>
       </c>
@@ -2801,7 +2825,7 @@
       </c>
       <c r="J5" s="22">
         <f>I5/$I$7</f>
-        <v>0.19298245614035087</v>
+        <v>0.1864406779661017</v>
       </c>
       <c r="K5" s="4">
         <v>20</v>
@@ -2825,7 +2849,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
@@ -2840,11 +2864,11 @@
       </c>
       <c r="I6" s="13">
         <f>SUMIF($C$2:$C$66,H6,$D$2:$D$66)</f>
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="J6" s="18">
         <f>I6/$I$7</f>
-        <v>0.31578947368421051</v>
+        <v>0.33898305084745761</v>
       </c>
       <c r="K6" s="4">
         <v>30</v>
@@ -2863,7 +2887,7 @@
       </c>
       <c r="V6" s="4"/>
     </row>
-    <row r="7" spans="1:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:22" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
         <v>96</v>
       </c>
@@ -2875,7 +2899,7 @@
       </c>
       <c r="I7" s="19">
         <f>SUM(I2:I6)</f>
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="Q7" s="19">
         <f>SUM(Q2:Q6)</f>
@@ -2883,7 +2907,7 @@
       </c>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:22" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:22" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>106</v>
       </c>
@@ -2894,7 +2918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="24" t="s">
         <v>107</v>
       </c>
@@ -2905,12 +2929,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="24" t="s">
         <v>171</v>
       </c>
@@ -2920,23 +2944,27 @@
       <c r="D11" s="13">
         <v>5</v>
       </c>
+      <c r="F11" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="40"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="24" t="s">
         <v>102</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="13">
-        <v>15</v>
+      <c r="D12" s="13"/>
+      <c r="F12" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="40"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
         <v>103</v>
       </c>
@@ -2944,25 +2972,29 @@
         <v>7</v>
       </c>
       <c r="D13" s="6">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="40"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" s="24" t="s">
         <v>99</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="13">
-        <v>15</v>
+      <c r="D14" s="13"/>
+      <c r="F14" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="40"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
         <v>104</v>
       </c>
@@ -2970,24 +3002,28 @@
         <v>7</v>
       </c>
       <c r="D15" s="6">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="40"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
         <v>100</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="13">
-        <v>15</v>
+      <c r="D16" s="13"/>
+      <c r="F16" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="24" t="s">
         <v>105</v>
       </c>
@@ -2995,11 +3031,14 @@
         <v>7</v>
       </c>
       <c r="D17" s="6">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
         <v>101</v>
       </c>
@@ -3007,11 +3046,14 @@
         <v>5</v>
       </c>
       <c r="D18" s="13">
-        <v>15</v>
+        <v>70</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
         <v>108</v>
       </c>
@@ -3019,11 +3061,14 @@
         <v>7</v>
       </c>
       <c r="D19" s="6">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>14</v>
       </c>
@@ -3033,9 +3078,12 @@
       <c r="D20" s="13">
         <v>5</v>
       </c>
+      <c r="F20" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
         <v>15</v>
       </c>
@@ -3043,11 +3091,14 @@
         <v>7</v>
       </c>
       <c r="D21" s="6">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="24" t="s">
         <v>16</v>
       </c>
@@ -3057,9 +3108,12 @@
       <c r="D22" s="13">
         <v>20</v>
       </c>
+      <c r="F22" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="24" t="s">
         <v>17</v>
       </c>
@@ -3067,11 +3121,14 @@
         <v>7</v>
       </c>
       <c r="D23" s="6">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="24" t="s">
         <v>6</v>
       </c>
@@ -3081,9 +3138,12 @@
       <c r="D24" s="15">
         <v>30</v>
       </c>
+      <c r="F24" s="5" t="s">
+        <v>184</v>
+      </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="24" t="s">
         <v>158</v>
       </c>
@@ -3094,7 +3154,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="29" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F29" s="5"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -3104,7 +3168,7 @@
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F30" s="5"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -3114,7 +3178,7 @@
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F31" s="5"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -3124,7 +3188,7 @@
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F32" s="5"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -3134,7 +3198,7 @@
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F33" s="5"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -3144,7 +3208,7 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F34" s="5"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -3154,7 +3218,7 @@
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F35" s="5"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -3164,7 +3228,7 @@
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F36" s="5"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -3174,7 +3238,7 @@
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
     </row>
-    <row r="37" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F37" s="5"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -3184,7 +3248,7 @@
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F38" s="5"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -3194,7 +3258,7 @@
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
     </row>
-    <row r="39" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F39" s="5"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -3204,7 +3268,7 @@
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
     </row>
-    <row r="40" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="24"/>
       <c r="F40" s="5"/>
       <c r="G40" s="3"/>
@@ -3215,7 +3279,7 @@
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
     </row>
-    <row r="41" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="24"/>
       <c r="F41" s="5"/>
       <c r="G41" s="3"/>
@@ -3226,7 +3290,7 @@
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="24"/>
       <c r="F42" s="5"/>
       <c r="G42" s="3"/>
@@ -3237,7 +3301,7 @@
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="24"/>
       <c r="F43" s="5"/>
       <c r="G43" s="3"/>
@@ -3248,7 +3312,7 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="24"/>
       <c r="F44" s="5"/>
       <c r="G44" s="3"/>
@@ -3259,7 +3323,7 @@
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="61" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="24"/>
       <c r="F61" s="5"/>
       <c r="G61" s="3"/>
@@ -3272,7 +3336,7 @@
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
     </row>
-    <row r="62" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="24"/>
       <c r="F62" s="5"/>
       <c r="G62" s="3"/>
@@ -3283,7 +3347,7 @@
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
     </row>
-    <row r="63" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="24"/>
       <c r="F63" s="5"/>
       <c r="G63" s="3"/>
@@ -3296,7 +3360,7 @@
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
     </row>
-    <row r="64" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="24"/>
       <c r="F64" s="5"/>
       <c r="G64" s="3"/>
@@ -3309,7 +3373,7 @@
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
     </row>
-    <row r="65" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="24"/>
       <c r="F65" s="5"/>
       <c r="G65" s="3"/>
@@ -3322,7 +3386,7 @@
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
     </row>
-    <row r="66" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="24"/>
       <c r="F66" s="5"/>
       <c r="G66" s="3"/>
@@ -3335,7 +3399,7 @@
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
     </row>
-    <row r="67" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="24"/>
       <c r="F67" s="5"/>
       <c r="G67" s="3"/>
@@ -3348,7 +3412,7 @@
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
     </row>
-    <row r="68" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="24"/>
       <c r="F68" s="5"/>
       <c r="G68" s="3"/>
@@ -3361,7 +3425,7 @@
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
     </row>
-    <row r="69" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="24"/>
       <c r="F69" s="5"/>
       <c r="G69" s="3"/>
@@ -3374,7 +3438,7 @@
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
     </row>
-    <row r="70" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="24"/>
       <c r="F70" s="5"/>
       <c r="G70" s="3"/>
@@ -3387,7 +3451,7 @@
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
     </row>
-    <row r="71" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="24"/>
       <c r="F71" s="5"/>
       <c r="G71" s="3"/>
@@ -3398,7 +3462,7 @@
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
     </row>
-    <row r="72" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="24"/>
       <c r="F72" s="5"/>
       <c r="G72" s="3"/>
@@ -3409,7 +3473,7 @@
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
     </row>
-    <row r="73" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="24"/>
       <c r="F73" s="5"/>
       <c r="G73" s="3"/>
@@ -3420,7 +3484,7 @@
       <c r="O73" s="3"/>
       <c r="P73" s="3"/>
     </row>
-    <row r="74" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="24"/>
       <c r="F74" s="5"/>
       <c r="G74" s="3"/>
@@ -3431,7 +3495,7 @@
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
     </row>
-    <row r="75" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="24"/>
       <c r="F75" s="5"/>
       <c r="G75" s="3"/>
@@ -3460,17 +3524,17 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25.9375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.25" style="44" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.625" customWidth="1"/>
     <col min="6" max="6" width="9" style="44"/>
-    <col min="7" max="7" width="12.9375" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>172</v>
       </c>
@@ -3482,7 +3546,7 @@
       </c>
       <c r="D1" s="45"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>180</v>
       </c>
@@ -3493,7 +3557,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>191</v>
       </c>
@@ -3516,7 +3580,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>33</v>
       </c>
@@ -3535,7 +3599,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>59</v>
       </c>
@@ -3558,7 +3622,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>56</v>
       </c>
@@ -3581,7 +3645,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>57</v>
       </c>
@@ -3592,7 +3656,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -3603,7 +3667,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -3614,37 +3678,37 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
post hw03 and OH
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161B88D2-0F2A-4A84-BBFE-E5E979DA3DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D14516-3F13-478E-8E8D-37790EB950BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1659,8 +1659,8 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="J6" s="52"/>
       <c r="K6" s="49"/>
-      <c r="L6" s="34" t="s">
+      <c r="L6" s="43" t="s">
         <v>65</v>
       </c>
       <c r="M6" s="34" t="s">
@@ -2376,7 +2376,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
       <c r="B25" s="25">
         <v>12.2</v>
       </c>

</xml_diff>

<commit_message>
fix lec2 link, add quiz 02 rebuild lkec03
</commit_message>
<xml_diff>
--- a/schedule_615.xlsx
+++ b/schedule_615.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\math615\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D14516-3F13-478E-8E8D-37790EB950BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE577547-325C-4F95-A739-BE1F12771034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4215" yWindow="1290" windowWidth="21600" windowHeight="11505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="weekly_schedule" sheetId="12" r:id="rId1"/>
@@ -668,9 +668,6 @@
     <t>canvas</t>
   </si>
   <si>
-    <t>lec02-asking_q</t>
-  </si>
-  <si>
     <t>Formulating research questions</t>
   </si>
   <si>
@@ -690,9 +687,6 @@
   </si>
   <si>
     <t>[HW01 Data Entry](hw01-data_entry.html)</t>
-  </si>
-  <si>
-    <t>[Quiz 02]()</t>
   </si>
   <si>
     <t>projecct</t>
@@ -714,6 +708,12 @@
   <si>
     <t>lec03a-workflow   
 lec03b-data_prep</t>
+  </si>
+  <si>
+    <t>[Quiz 02](https://forms.gle/2hPjWMkGpiXuZg1S6)</t>
+  </si>
+  <si>
+    <t>lec02-asking_q</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1060,7 @@
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="77" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1224,6 +1224,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1658,9 +1661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C53430-DF90-419A-8B50-2697098F702F}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1713,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L1" s="46" t="s">
         <v>42</v>
@@ -1751,7 +1754,7 @@
         <v>29</v>
       </c>
       <c r="K2" s="49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L2" s="43" t="s">
         <v>43</v>
@@ -1784,13 +1787,13 @@
       </c>
       <c r="J3" s="35"/>
       <c r="K3" s="51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L3" s="43" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M3" s="43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
@@ -1829,7 +1832,7 @@
         <v>56</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>48</v>
@@ -1838,14 +1841,14 @@
         <v>118</v>
       </c>
       <c r="H5" s="43" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="I5" s="50" t="s">
         <v>49</v>
       </c>
       <c r="J5" s="43"/>
       <c r="K5" s="51" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L5" s="43" t="s">
         <v>64</v>
@@ -1872,18 +1875,18 @@
         <v>50</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>207</v>
-      </c>
-      <c r="I6" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>204</v>
       </c>
       <c r="J6" s="52"/>
       <c r="K6" s="49"/>
       <c r="L6" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="M6" s="34" t="s">
-        <v>201</v>
+      <c r="M6" s="43" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1893,36 +1896,37 @@
       <c r="B7" s="29">
         <v>3.1</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="48">
         <v>43711</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="57"/>
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="29">
         <v>3.2</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="48">
         <v>43713</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35" t="s">
+      <c r="D8" s="57"/>
+      <c r="E8" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="34"/>
+      <c r="G8" s="43"/>
       <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
@@ -3554,7 +3558,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3568,7 +3572,7 @@
         <v>189</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>188</v>
@@ -3591,7 +3595,7 @@
         <v>174</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E5" s="41"/>
       <c r="F5" s="45"/>
@@ -3610,7 +3614,7 @@
         <v>175</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E6" s="41" t="s">
         <v>185</v>
@@ -3633,13 +3637,13 @@
         <v>176</v>
       </c>
       <c r="D7" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="E7" s="41" t="s">
-        <v>205</v>
-      </c>
       <c r="F7" s="45" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G7" s="45" t="s">
         <v>184</v>

</xml_diff>